<commit_message>
Setting screen size for raspberry pi screen
</commit_message>
<xml_diff>
--- a/Pokemonstuff2.xlsx
+++ b/Pokemonstuff2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f5c6edd2c1ca723/Documents/pokedex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2249" documentId="8_{6427532F-30D5-4B25-B377-222758C656F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B2AADBF-047F-4CFF-83D2-85FE05ACA1CA}"/>
+  <xr:revisionPtr revIDLastSave="2871" documentId="8_{6427532F-30D5-4B25-B377-222758C656F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF48F1B5-8045-44B2-90F7-9DB590802970}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemonstuff" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6137" uniqueCount="3733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="4023">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -11553,6 +11553,892 @@
   </si>
   <si>
     <t>Terapagos Stellar Form</t>
+  </si>
+  <si>
+    <t>Duck Pokémon</t>
+  </si>
+  <si>
+    <t>19.6 kg</t>
+  </si>
+  <si>
+    <t>Damp
+Cloud Nine
+Swift Swim</t>
+  </si>
+  <si>
+    <t>Field, Water 1</t>
+  </si>
+  <si>
+    <t>Level 33</t>
+  </si>
+  <si>
+    <t>While lulling its enemies with its vacant look, this wily POKéMON will use psychokinetic powers.</t>
+  </si>
+  <si>
+    <t>Always tormented by headaches. It uses psychic powers, but it is not known if it intends to do so.</t>
+  </si>
+  <si>
+    <t>It has mystical powers but doesn’t recall that it has used them. That is why it always looks puzzled.</t>
+  </si>
+  <si>
+    <t>If its chronic headache peaks, it may exhibit odd powers. It seems unable to recall such an episode.</t>
+  </si>
+  <si>
+    <t>The only time it can use its psychic power is when its sleeping brain cells happen to wake.</t>
+  </si>
+  <si>
+    <t>PSYDUCK uses a mysterious power. When it does so, this POKéMON generates brain waves that are supposedly only seen in sleepers. This discovery spurred controversy among scholars.</t>
+  </si>
+  <si>
+    <t>If it uses its mysterious power, PSYDUCK can’t remember having done so. It apparently can’t form a memory of such an event because it goes into an altered state that is much like deep sleep.</t>
+  </si>
+  <si>
+    <t>It is constantly wracked by a headache. When the headache turns intense, it begins using mysterious powers.</t>
+  </si>
+  <si>
+    <t>When its headache intensifies, it starts using strange powers. However, it has no recollection of its powers, so it always looks befuddled and bewildered.</t>
+  </si>
+  <si>
+    <t>If its usual headache worsens, it starts exhibiting odd powers. It can’t remember doing so, however.</t>
+  </si>
+  <si>
+    <t>It never remembers using its odd powers, so it always tilts its head in puzzlement.</t>
+  </si>
+  <si>
+    <t>Overwhelmed by enigmatic abilities, it suffers a constant headache. It sometimes uses mysterious powers.</t>
+  </si>
+  <si>
+    <t>When headaches stimulate its brain cells, which are usually inactive, it can use a mysterious power.</t>
+  </si>
+  <si>
+    <t>Psyduck uses a mysterious power. When it does so, this Pokémon generates brain waves that are supposedly only seen in sleepers. This discovery spurred controversy among scholars.</t>
+  </si>
+  <si>
+    <t>If it uses its mysterious power, Psyduck can’t remember having done so. It apparently can’t form a memory of such an event because it goes into an altered state that is much like deep sleep.</t>
+  </si>
+  <si>
+    <t>As a result of headaches so fierce they cause it to cry, it sometimes uses psychokinesis without meaning to.</t>
+  </si>
+  <si>
+    <t>This Pokémon is troubled by constant headaches. The more pain it’s in, the more powerful its psychokinesis becomes.</t>
+  </si>
+  <si>
+    <t>Using psychokinesis gives it a headache, so it normally passes the time spacing out and doing as little as possible.</t>
+  </si>
+  <si>
+    <t>It has been found that its brain cells are 10 times more active when Psyduck is experiencing a headache.</t>
+  </si>
+  <si>
+    <t>Always tormented by headaches. It uses psychic powers, but whether it intends to do so is not known.</t>
+  </si>
+  <si>
+    <t>Psyduck is constantly beset by headaches. If the Pokémon lets its strange power erupt, apparently the pain subsides for a while.</t>
+  </si>
+  <si>
+    <t>As Psyduck gets stressed out, its headache gets progressively worse. It uses intense psychic energy to overwhelm those around it.</t>
+  </si>
+  <si>
+    <t>Suffers perpetual headaches. If the agony grows too great, Psyduck’s latent power erupts, contrary to Psyduck’s intent. Ergo, I am exploring ways to ease the pain.</t>
+  </si>
+  <si>
+    <t>76.6 kg</t>
+  </si>
+  <si>
+    <t>Often seen swimming elegantly by lake shores. It is often mistaken for the Japanese monster, Kappa.</t>
+  </si>
+  <si>
+    <t>Its slim and long limbs end in broad flippers. They are used for swimming gracefully in lakes.</t>
+  </si>
+  <si>
+    <t>When it swims at full speed using its long, webbed limbs, its forehead somehow begins to glow.</t>
+  </si>
+  <si>
+    <t>It appears by waterways at dusk. It may use telekinetic powers if its forehead glows mysteriously.</t>
+  </si>
+  <si>
+    <t>It swims gracefully along on the quiet, slow-moving rivers and lakes of which it is so fond.</t>
+  </si>
+  <si>
+    <t>The webbed flippers on its forelegs and hind legs and the streamlined body of GOLDUCK give it frightening speed. This POKéMON is definitely much faster than even the most athletic swimmer.</t>
+  </si>
+  <si>
+    <t>GOLDUCK is the fastest swimmer among all POKéMON. It swims effortlessly, even in a rough, stormy sea. It sometimes rescues people from wrecked ships floundering in high seas.</t>
+  </si>
+  <si>
+    <t>The forelegs are webbed, helping to make it an adept swimmer. It can be seen swimming elegantly in lakes, etc.</t>
+  </si>
+  <si>
+    <t>Often seen swimming elegantly by lakeshores. It is often mistaken for the Japanese monster Kappa.</t>
+  </si>
+  <si>
+    <t>A GOLDUCK is an adept swimmer. It sometimes joins competitive swimmers in training. It uses psychic powers when its forehead shimmers with light.</t>
+  </si>
+  <si>
+    <t>A Pokémon that lives in lakes. It swims faster than any human swimming champion.</t>
+  </si>
+  <si>
+    <t>The flippers of its well-developed limbs give it shocking speed. It is the best swimmer among Pokémon.</t>
+  </si>
+  <si>
+    <t>It is seen swimming dynamically and elegantly using its well-developed limbs and flippers.</t>
+  </si>
+  <si>
+    <t>When its forehead shines mysteriously, Golduck can use the full extent of its power.</t>
+  </si>
+  <si>
+    <t>The webbed flippers on its forelegs and hind legs and the streamlined body of Golduck give it frightening speed. This Pokémon is definitely much faster than even the most athletic swimmer.</t>
+  </si>
+  <si>
+    <t>Golduck is the fastest swimmer among all Pokémon. It swims effortlessly, even in a rough, stormy sea. It sometimes rescues people from wrecked ships floundering in high seas.</t>
+  </si>
+  <si>
+    <t>It is said that the red part of its forehead grants supernatural powers to those who possess one, so it was over-hunted in the past.</t>
+  </si>
+  <si>
+    <t>It swims along the banks of lakes and catches fish Pokémon. It takes them to the shore and quietly eats them up.</t>
+  </si>
+  <si>
+    <t>Even fast-swimming fish Pokémon can be disabled by Golduck. It brings them to a standstill and seizes them.</t>
+  </si>
+  <si>
+    <t>A professional swimmer, it can continue swimming for two days straight by waving its long tail skillfully.</t>
+  </si>
+  <si>
+    <t>Its long, slim limbs end in broad flippers. They are used for swimming gracefully in lakes.</t>
+  </si>
+  <si>
+    <t>This Pokémon lives in gently flowing rivers. It paddles through the water with its long limbs, putting its graceful swimming skills on display.</t>
+  </si>
+  <si>
+    <t>Old tales tell of Golduck punishing those that defiled its river. The guilty were dragged into the water and taken away.</t>
+  </si>
+  <si>
+    <t>This Pokémon lives in lakes. It swims faster than any world-class swimmer.</t>
+  </si>
+  <si>
+    <t>Its body is strong, and it has webbing on its hands and feet. Golduck can swim easily through rough seas, clawing its way through the high waves.</t>
+  </si>
+  <si>
+    <t>Pig Monkey Pokémon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 m </t>
+  </si>
+  <si>
+    <t>28.0 kg</t>
+  </si>
+  <si>
+    <t>Vital Spirit
+Anger Point
+Defiant</t>
+  </si>
+  <si>
+    <t>Extremely quick to anger. It could be docile one moment then thrashing away the next instant.</t>
+  </si>
+  <si>
+    <t>An agile POKéMON that lives in trees. It angers easily and will not hesitate to attack anything.</t>
+  </si>
+  <si>
+    <t>It is extremely ill-tempered. Groups of them will attack any handy target for no reason.</t>
+  </si>
+  <si>
+    <t>It’s unsafe to approach if it gets violently enraged for no reason and can’t distinguish friends from foes.</t>
+  </si>
+  <si>
+    <t>It lives in groups in the treetops. If it loses sight of its group, it becomes infuriated by its loneliness.</t>
+  </si>
+  <si>
+    <t>When MANKEY starts shaking and its nasal breathing turns rough, it’s a sure sign that it is becoming angry. However, because it goes into a towering rage almost instantly, it is impossible for anyone to flee its wrath.</t>
+  </si>
+  <si>
+    <t>Light and agile on its feet, and ferocious in temperament. When angered, it flies into an uncontrollable frenzy.</t>
+  </si>
+  <si>
+    <t>Extremely quick to anger. It could be docile one moment, then thrashing away the next instant.</t>
+  </si>
+  <si>
+    <t>When it starts shaking and its nasal breathing turns rough, it’s a sure sign of anger. However, since this happens instantly, there is no time to flee.</t>
+  </si>
+  <si>
+    <t>It lives in treetop colonies. If one becomes enraged, the whole colony rampages for no reason.</t>
+  </si>
+  <si>
+    <t>When Mankey starts shaking and its nasal breathing turns rough, it’s a sure sign that it is becoming angry. However, because it goes into a towering rage almost instantly, it is impossible for anyone to flee its wrath.</t>
+  </si>
+  <si>
+    <t>It can spontaneously become enraged. Everyone near it clears out as it rampages, and the resulting loneliness makes it angrier still.</t>
+  </si>
+  <si>
+    <t>Its raging tires it out and causes it to fall asleep, but the anger resonating in its dreams causes it to wake up—which infuriates it all over again.</t>
+  </si>
+  <si>
+    <t>The smallest of things could cause it to lose its temper. Because it doesn’t hold in its stress, this Pokémon can live a long time.</t>
+  </si>
+  <si>
+    <t>If one gets angry, all the others around it will get angry, so silence is a rare visitor in a troop of Mankey.</t>
+  </si>
+  <si>
+    <t>An agile Pokémon that lives in trees. It angers easily and will not hesitate to attack anything.</t>
+  </si>
+  <si>
+    <t>It lives in treetop colonies. If one member of the group becomes enraged, the whole colony rampages for no reason.</t>
+  </si>
+  <si>
+    <t>It is extremely quick to anger. It could be docile one moment, then thrashing away the next instant.</t>
+  </si>
+  <si>
+    <t>Always furious and tenacious to boot. It will not abandon chasing its quarry until it is caught.</t>
+  </si>
+  <si>
+    <t>It stops being angry only when nobody else is around. To view this moment is very difficult.</t>
+  </si>
+  <si>
+    <t>If approached while asleep, it may awaken and angrily give chase in a groggy state of semi-sleep.</t>
+  </si>
+  <si>
+    <t>It becomes wildly furious if it even senses someone looking at it. It chases anyone that meets its glare.</t>
+  </si>
+  <si>
+    <t>It will beat up anyone who makes it mad, even if it has to chase them until the end of the world.</t>
+  </si>
+  <si>
+    <t>When PRIMEAPE becomes furious, its blood circulation is boosted. In turn, its muscles are made even stronger. However, it also becomes much less intelligent at the same time.</t>
+  </si>
+  <si>
+    <t>It is always outrageously furious. If it gives chase, it will tenaciously track the target no matter how far.</t>
+  </si>
+  <si>
+    <t>Always furious and tenacious to boot. It will not abandon chasing its quarry until it catches up.</t>
+  </si>
+  <si>
+    <t>When it becomes furious, its blood circulation becomes more robust, and its muscles are made stronger. But it also becomes much less intelligent.</t>
+  </si>
+  <si>
+    <t>It grows angry if you see its eyes and gets angrier if you run. If you beat it, it gets even madder.</t>
+  </si>
+  <si>
+    <t>When Primeape becomes furious, its blood circulation is boosted. In turn, its muscles are made even stronger. However, it also becomes much less intelligent at the same time.</t>
+  </si>
+  <si>
+    <t>It has been known to become so angry that it dies as a result. Its face looks peaceful in death, however.</t>
+  </si>
+  <si>
+    <t>Some researchers theorize that Primeape remains angry even when inside a Poké Ball.</t>
+  </si>
+  <si>
+    <t>It will never forgive opponents who have angered it. Even after it has beaten them down until they can’t move, it never ever forgives.</t>
+  </si>
+  <si>
+    <t>The blood vessels in its brain are sturdier than those of other Pokémon, so it can stay healthy despite its constant raging.</t>
+  </si>
+  <si>
+    <t>It becomes angry if it sees an opponent’s eyes and gets angrier if the opponent runs. Even after it beats the opponent, it is still angry.</t>
+  </si>
+  <si>
+    <t>Puppy Pokémon</t>
+  </si>
+  <si>
+    <t>Intimidate
+Flash Fire
+Justified</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>75% male
+25% female</t>
+  </si>
+  <si>
+    <t>Scout Pokémon</t>
+  </si>
+  <si>
+    <t>22.7 kg</t>
+  </si>
+  <si>
+    <t>Intimidate
+Flash Fire
+Rock Head</t>
+  </si>
+  <si>
+    <t>Very protective of its territory. It will bark and bite to repel intruders from its space.</t>
+  </si>
+  <si>
+    <t>A POKéMON with a friendly nature. However, it will bark fiercely at anything invading its territory.</t>
+  </si>
+  <si>
+    <t>It has a brave and trustworthy nature. It fearlessly stands up to bigger and stronger foes.</t>
+  </si>
+  <si>
+    <t>Extremely loyal, it will fearlessly bark at any opponent to protect its own trainer from harm.</t>
+  </si>
+  <si>
+    <t>It controls a big territory. If it detects an unknown smell, it roars loudly to force out the intruder.</t>
+  </si>
+  <si>
+    <t>GROWLITHE has a superb sense of smell. Once it smells anything, this POKéMON won’t forget the scent, no matter what. It uses its advanced olfactory sense to determine the emotions of other living things.</t>
+  </si>
+  <si>
+    <t>Very friendly and faithful to people. It will try to repel enemies by barking and biting.</t>
+  </si>
+  <si>
+    <t>It is very protective of its territory. It will bark and bite to repel intruders from its space.</t>
+  </si>
+  <si>
+    <t>Its superb sense of smell ensures that this POKéMON won’t forget any scent, no matter what. It uses its sense of smell to detect the emotions of others.</t>
+  </si>
+  <si>
+    <t>A Pokémon with a loyal nature. It will remain motionless until it is given an order by its Trainer.</t>
+  </si>
+  <si>
+    <t>Extremely loyal, it will fearlessly bark at any opponent to protect its own Trainer from harm.</t>
+  </si>
+  <si>
+    <t>Extremely loyal to its Trainer, it will bark at those who approach the Trainer unexpectedly and run them out of town.</t>
+  </si>
+  <si>
+    <t>Growlithe has a superb sense of smell. Once it smells anything, this Pokémon won’t forget the scent, no matter what. It uses its advanced olfactory sense to determine the emotions of other living things.</t>
+  </si>
+  <si>
+    <t>It’s both clever and loyal, but if a stranger tries to invade its territory, it barks threateningly.</t>
+  </si>
+  <si>
+    <t>It looks cute, but when you approach another Trainer’s Growlithe, it will bark at you and bite.</t>
+  </si>
+  <si>
+    <t>While it’s quite friendly toward humans once it’s grown used to them, in the wild it must be quite fierce to defend its territory from Rockruff.</t>
+  </si>
+  <si>
+    <t>It has lived alongside humans since ages ago. Its bones have been found in excavations of ruins from the Stone Age.</t>
+  </si>
+  <si>
+    <t>A Pokémon with a friendly nature. However, it will bark fiercely at anything invading its territory.</t>
+  </si>
+  <si>
+    <t>It is a Pokémon with a loyal nature. It will remain motionless until it is given an order by its Trainer.</t>
+  </si>
+  <si>
+    <t>It’s very friendly and faithful to people. It will try to repel enemies by barking and biting.</t>
+  </si>
+  <si>
+    <t>They patrol their territory in pairs. I believe the igneous rock components in the fur of this species are the result of volcanic activity in its habitat.</t>
+  </si>
+  <si>
+    <t>Legendary Pokémon</t>
+  </si>
+  <si>
+    <t>1.9 m</t>
+  </si>
+  <si>
+    <t>155.0 kg</t>
+  </si>
+  <si>
+    <t>168.0 kg</t>
+  </si>
+  <si>
+    <t>A POKéMON that has been admired since the past for its beauty. It runs agilely as if on wings.</t>
+  </si>
+  <si>
+    <t>This legendary Chinese POKEMON is considered magnificent. Many people are enchanted by its grand mane.</t>
+  </si>
+  <si>
+    <t>Its magnificent bark conveys a sense of majesty. Anyone hearing it can’t help but grovel before it.</t>
+  </si>
+  <si>
+    <t>An ancient picture scroll shows that people were attracted to its movement as it ran through prairies.</t>
+  </si>
+  <si>
+    <t>ARCANINE is known for its high speed. It is said to be capable of running over 6,200 miles in a single day and night. The fire that blazes wildly within this POKéMON’s body is its source of power.</t>
+  </si>
+  <si>
+    <t>A POKéMON that is described in Chinese legends. It is said to race at an unbelievable speed.</t>
+  </si>
+  <si>
+    <t>A POKéMON that has long been admired for its beauty. It runs agilely as if on wings.</t>
+  </si>
+  <si>
+    <t>This fleet-footed POKéMON is said to run over 6,200 miles in a single day and night. The fire that blazes wildly within its body is its source of power.</t>
+  </si>
+  <si>
+    <t>Its proud and regal appearance has captured the hearts of people since long ago.</t>
+  </si>
+  <si>
+    <t>This legendary Chinese Pokémon is considered magnificent. Many people are enchanted by its grand mane.</t>
+  </si>
+  <si>
+    <t>The sight of it running over 6,200 miles in a single day and night has captivated many people.</t>
+  </si>
+  <si>
+    <t>A Pokémon that has long been admired for its beauty. It runs agilely as if on wings.</t>
+  </si>
+  <si>
+    <t>Arcanine is known for its high speed. It is said to be capable of running over 6,200 miles in a single day and night. The fire that blazes wildly within this Pokémon’s body is its source of power.</t>
+  </si>
+  <si>
+    <t>Overflowing with beauty and majesty, this strong Pokémon appears in ancient Eastern folklore.</t>
+  </si>
+  <si>
+    <t>The fire burning inside its body serves as the energy to fuel it as it runs great distances. It appears in many legends.</t>
+  </si>
+  <si>
+    <t>Legends tell of its fighting alongside a general and conquering a whole country.</t>
+  </si>
+  <si>
+    <t>There are so many old tales about them that they’re called legendary Pokémon, but there are way more of them around than you’d expect.</t>
+  </si>
+  <si>
+    <t>A legendary Pokémon in the East. Many people are charmed by the grace and beauty of its running.</t>
+  </si>
+  <si>
+    <t>An ancient picture scroll shows that people were captivated by its movement as it ran through prairies.</t>
+  </si>
+  <si>
+    <t>Snaps at its foes with fangs cloaked in blazing flame. Despite its bulk, it deftly feints every which way, leading opponents on a deceptively merry chase as it all but dances around them.</t>
+  </si>
+  <si>
+    <t>Tadpole Pokémon</t>
+  </si>
+  <si>
+    <t>12.4 kg</t>
+  </si>
+  <si>
+    <t>Water Absorb
+Damp
+Swift Swim</t>
+  </si>
+  <si>
+    <t>Water 1</t>
+  </si>
+  <si>
+    <t>Level 25</t>
+  </si>
+  <si>
+    <t>Water Stone
+Kings Rock</t>
+  </si>
+  <si>
+    <t>Its newly grown legs prevent it from running. It appears to prefer swimming than trying to stand.</t>
+  </si>
+  <si>
+    <t>The direction of the spiral on the belly differs by area. It is more adept at swimming than walking.</t>
+  </si>
+  <si>
+    <t>Because it is inept at walking on its newly grown legs, it always swims around in water.</t>
+  </si>
+  <si>
+    <t>The direction of its belly spiral differs by area. The equator is thought to have an effect on this.</t>
+  </si>
+  <si>
+    <t>The swirl on its belly is its insides showing through the skin. It looks clearer after it eats.</t>
+  </si>
+  <si>
+    <t>POLIWAG has a very thin skin. It is possible to see the POKéMON’s spiral innards right through the skin. Despite its thinness, however, the skin is also very flexible. Even sharp fangs bounce right off it.</t>
+  </si>
+  <si>
+    <t>Its slick black skin is thin and damp. A part of its internal organs can be seen through the skin as a spiral pattern.</t>
+  </si>
+  <si>
+    <t>Its newly grown legs prevent it from walking well. It appears to prefer swimming over walking.</t>
+  </si>
+  <si>
+    <t>It is possible to see this POKéMON’s spiral innards right through its thin skin. However, the skin is also very flexible. Even sharp fangs bounce right off it.</t>
+  </si>
+  <si>
+    <t>Its skin is so thin, its internal organs are visible. It has trouble walking on its newly grown feet.</t>
+  </si>
+  <si>
+    <t>Poliwag has a very thin skin. It is possible to see the Pokémon’s spiral innards right through the skin. Despite its thinness, however, the skin is also very flexible. Even sharp fangs bounce right off it.</t>
+  </si>
+  <si>
+    <t>The swirl on its belly is its internal organs showing through. If the swirl is tinged white, that means it’s affected by some disease.</t>
+  </si>
+  <si>
+    <t>It’s still not very good at walking. Its Trainers should train this Pokémon to walk every day.</t>
+  </si>
+  <si>
+    <t>Despite the danger, it wants to come up on land. So it does its best to waddle along, but when an enemy finds it, it rushes back to the water.</t>
+  </si>
+  <si>
+    <t>The direction of the swirl on their stomachs differs depending on where they live. Poliwag aficionados can tell them apart at a glance.</t>
+  </si>
+  <si>
+    <t>For Poliwag, swimming is easier than walking. The swirl pattern on its belly is actually part of the Pokémon’s innards showing through the skin.</t>
+  </si>
+  <si>
+    <t>In rivers with fast-flowing water, this Pokémon will cling to a rock by using its thick lips, which act like a suction cup.</t>
+  </si>
+  <si>
+    <t>Capable of living in or out of water. When out of water, it sweats to keep its body slimy.</t>
+  </si>
+  <si>
+    <t>Under attack, it uses its belly spiral to put the foe to sleep. It then makes its escape.</t>
+  </si>
+  <si>
+    <t>The swirl on its belly subtly undulates. Staring at it may gradually cause drowsiness.</t>
+  </si>
+  <si>
+    <t>The skin on most of its body is moist. However, the skin on its belly spiral feels smooth.</t>
+  </si>
+  <si>
+    <t>Though it is skilled at walking, it prefers to live underwater where there is less danger.</t>
+  </si>
+  <si>
+    <t>The surface of POLIWHIRL’s body is always wet and slick with an oily fluid. Because of this greasy covering, it can easily slip and slide out of the clutches of any enemy in battle.</t>
+  </si>
+  <si>
+    <t>Its two legs are well developed. Even though it can live on the ground, it prefers living in water.</t>
+  </si>
+  <si>
+    <t>It can live in or out of water. When out of water, it constantly sweats to keep its body slimy.</t>
+  </si>
+  <si>
+    <t>Its body surface is always wet and slick with an oily fluid. Because of this greasy covering, it can easily slip and slide out of the clutches of any enemy in battle.</t>
+  </si>
+  <si>
+    <t>The spiral pattern on its belly subtly undulates. Staring at it gradually causes drowsiness.</t>
+  </si>
+  <si>
+    <t>The surface of Poliwhirl’s body is always wet and slick with a slimy fluid. Because of this slippery covering, it can easily slip and slide out of the clutches of any enemy in battle.</t>
+  </si>
+  <si>
+    <t>Although it can live on land, it prefers to stay in the water, where it has fewer natural enemies.</t>
+  </si>
+  <si>
+    <t>It marches over the land in search of bug Pokémon to eat. Then it takes them underwater so it can dine on them where it’s safe.</t>
+  </si>
+  <si>
+    <t>Although it has become capable of living on land, it spends its time in the water, where its prey, fish Pokémon, are plentiful.</t>
+  </si>
+  <si>
+    <t>Its health suffers when its skin dries out, so be sure to moisturize it diligently.</t>
+  </si>
+  <si>
+    <t>Staring at the swirl on its belly causes drowsiness. This trait of Poliwhirl’s has been used in place of lullabies to get children to go to sleep.</t>
+  </si>
+  <si>
+    <t>This Pokémon’s sweat is a slimy mucus. When captured, Poliwhirl can slither from its enemies’ grasp and escape.</t>
+  </si>
+  <si>
+    <t>54.0 kg</t>
+  </si>
+  <si>
+    <t>An adept swimmer at both the front crawl and breast stroke. Easily overtakes the best human swimmers.</t>
+  </si>
+  <si>
+    <t>Swims powerfully using all the muscles in its body. It can even overtake champion swimmers.</t>
+  </si>
+  <si>
+    <t>This strong and skilled swimmer is even capable of crossing the Pacific Ocean just by kicking.</t>
+  </si>
+  <si>
+    <t>Although an energetic, skilled swimmer that uses all of its muscles, it lives on dry land.</t>
+  </si>
+  <si>
+    <t>It can use its well-developed arms and legs to run on the surface of the water for a split second.</t>
+  </si>
+  <si>
+    <t>POLIWRATH’s highly developed, brawny muscles never grow fatigued, however much it exercises. It is so tirelessly strong, this POKéMON can swim back and forth across the Pacific Ocean without effort.</t>
+  </si>
+  <si>
+    <t>An adept swimmer, it knows the front crawl, butterfly, and more. It is faster than the best human swimmers.</t>
+  </si>
+  <si>
+    <t>A swimmer adept at both the front crawl and breaststroke. Easily overtakes the best human swimmers.</t>
+  </si>
+  <si>
+    <t>Its highly developed muscles never grow fatigued, however much it exercises. This POKéMON can swim back and forth across the Pacific Ocean without effort.</t>
+  </si>
+  <si>
+    <t>With its extremely tough muscles, it can keep swimming in the Pacific Ocean without resting.</t>
+  </si>
+  <si>
+    <t>Poliwrath’s highly developed, brawny muscles never grow fatigued, however much it exercises. It is so tirelessly strong, this Pokémon can swim back and forth across the ocean without effort.</t>
+  </si>
+  <si>
+    <t>Poliwrath in the Alola region are strong swimmers that use the breaststroke. Many children learn to swim by imitating Poliwrath.</t>
+  </si>
+  <si>
+    <t>Its percentage of body fat is nearly zero. Its body is entirely muscle, which makes it heavy and forces its swimming prowess to develop.</t>
+  </si>
+  <si>
+    <t>It’s quite a gifted swimmer, even among Water-type Pokémon, but it normally spends its time on land.</t>
+  </si>
+  <si>
+    <t>The muscles it has developed through swimming are thick and powerful. When it lands a square punch, it can turn huge boulders to dust.</t>
+  </si>
+  <si>
+    <t>Swims powerfully using all the muscles in its body. It can even overtake world-class swimmers.</t>
+  </si>
+  <si>
+    <t>Its body is solid muscle. When swimming through cold seas, Poliwrath uses its impressive arms to smash through drift ice and plow forward.</t>
+  </si>
+  <si>
+    <t>Poliwrath is skilled at both swimming and martial arts. It uses its well-trained arms to dish out powerful punches.</t>
+  </si>
+  <si>
+    <t>With its extremely tough muscles, it could keep swimming in the Pacific Ocean without resting.</t>
+  </si>
+  <si>
+    <t>Psi Pokémon</t>
+  </si>
+  <si>
+    <t>Synchronize
+Inner Focus
+Magic Guard</t>
+  </si>
+  <si>
+    <t>Human_Like</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Using its ability to read minds, it will identify impending danger and TELEPORT to safety.</t>
+  </si>
+  <si>
+    <t>Sleeps 18 hours a day. If it senses danger, it will teleport itself to safety even as it sleeps.</t>
+  </si>
+  <si>
+    <t>It senses impending attacks and TELEPORTS away to safety before the actual attacks can strike.</t>
+  </si>
+  <si>
+    <t>If it decides to TELEPORT randomly, it creates the illusion that it has created copies of itself.</t>
+  </si>
+  <si>
+    <t>It hypnotizes itself so that it can teleport away when it senses danger, even if it is asleep.</t>
+  </si>
+  <si>
+    <t>ABRA sleeps for eighteen hours a day. However, it can sense the presence of foes even while it is sleeping. In such a situation, this POKéMON immediately teleports to safety.</t>
+  </si>
+  <si>
+    <t>ABRA needs to sleep for eighteen hours a day. If it doesn’t, this POKéMON loses its ability to use telekinetic powers. If it is attacked, ABRA escapes using TELEPORT while it is still sleeping.</t>
+  </si>
+  <si>
+    <t>It sleeps for 18 hours a day. It uses a variety of extrasensory powers even while asleep.</t>
+  </si>
+  <si>
+    <t>Using its ability to read minds, it will sense impending danger and TELEPORT to safety.</t>
+  </si>
+  <si>
+    <t>A POKéMON that sleeps 18 hours a day. Observation revealed that it uses TELEPORT to change its location once every hour.</t>
+  </si>
+  <si>
+    <t>It sleeps for 18 hours a day. Even when awake, it teleports itself while remaining seated.</t>
+  </si>
+  <si>
+    <t>Even while asleep, it maintains a telepathic radar. It teleports when it is threatened.</t>
+  </si>
+  <si>
+    <t>Using its psychic power is such a strain on its brain that it needs to sleep for 18 hours a day.</t>
+  </si>
+  <si>
+    <t>It senses impending attacks and teleports away to safety before the actual attacks can strike.</t>
+  </si>
+  <si>
+    <t>If it decides to teleport randomly, it evokes the illusion that it has created copies of itself.</t>
+  </si>
+  <si>
+    <t>Abra sleeps for eighteen hours a day. However, it can sense the presence of foes even while it is sleeping. In such a situation, this Pokémon immediately teleports to safety.</t>
+  </si>
+  <si>
+    <t>Abra needs to sleep for eighteen hours a day. If it doesn’t, this Pokémon loses its ability to use telekinetic powers. If it is attacked, Abra escapes using Teleport while it is still sleeping.</t>
+  </si>
+  <si>
+    <t>It sleeps 18 hours a day. Even while sleeping, it will teleport itself to treetops and pick and eat berries there.</t>
+  </si>
+  <si>
+    <t>It can teleport itself to safety while it’s asleep, but when it wakes, it doesn’t know where it is, so it panics.</t>
+  </si>
+  <si>
+    <t>It uses various psychic powers even while it’s sleeping, so you can’t tell whether or not it’s awake.</t>
+  </si>
+  <si>
+    <t>It can read others’ minds and will teleport away when danger approaches. You must clear your mind if you want to catch it.</t>
+  </si>
+  <si>
+    <t>This Pokémon uses its psychic powers while it sleeps. The contents of Abra’s dreams affect the powers that the Pokémon wields.</t>
+  </si>
+  <si>
+    <t>Abra can teleport in its sleep. Apparently the more deeply Abra sleeps, the farther its teleportations go.</t>
+  </si>
+  <si>
+    <t>Spends 18 hours of the day sleeping. Even while asleep, Abra can control its psychic powers—should danger approach, the Pokémon will simply teleport away.</t>
+  </si>
+  <si>
+    <t>56.5 kg</t>
+  </si>
+  <si>
+    <t>It emits special alpha waves from its body that induce headaches just by being close by.</t>
+  </si>
+  <si>
+    <t>Many odd things happen if this POKéMON is close by. For example, it makes clocks run backwards.</t>
+  </si>
+  <si>
+    <t>It possesses strong spiritual power. The more danger it faces, the stronger its psychic power.</t>
+  </si>
+  <si>
+    <t>If it uses its abilities, it emits special alpha waves that cause machines to malfunction.</t>
+  </si>
+  <si>
+    <t>When it closes its eyes, twice as many alpha particles come out of the surface of its body.</t>
+  </si>
+  <si>
+    <t>KADABRA emits a peculiar alpha wave if it develops a headache. Only those people with a particularly strong psyche can hope to become a TRAINER of this POKéMON.</t>
+  </si>
+  <si>
+    <t>KADABRA holds a silver spoon in its hand. The spoon is used to amplify the alpha waves in its brain. Without the spoon, the POKéMON is said to be limited to half the usual amount of its telekinetic powers.</t>
+  </si>
+  <si>
+    <t>It happened one morning - a boy with extrasensory powers awoke in bed transformed into KADABRA.</t>
+  </si>
+  <si>
+    <t>It emits special alpha waves from its body that induce headaches just by being close.</t>
+  </si>
+  <si>
+    <t>It is rumored that a boy with psychic abilities suddenly transformed into KADABRA while he was assisting research into extrasensory powers.</t>
+  </si>
+  <si>
+    <t>If one is nearby, an eerie shadow appears on TV screens. Seeing the shadow is said to bring bad luck.</t>
+  </si>
+  <si>
+    <t>When it uses its psychic power, it emits strong ha waves that can ruin precision devices.</t>
+  </si>
+  <si>
+    <t>It stares at its silver spoon to focus its mind. It emits more alpha waves while doing so.</t>
+  </si>
+  <si>
+    <t>When it uses its psychic power, it emits strong alpha waves that can ruin precision devices.</t>
+  </si>
+  <si>
+    <t>Kadabra emits a peculiar alpha wave if it develops a headache. Only those people with a particularly strong psyche can hope to become a Trainer of this Pokémon.</t>
+  </si>
+  <si>
+    <t>Kadabra holds a silver spoon in its hand. The spoon is used to amplify the alpha waves in its brain. Without the spoon, the Pokémon is said to be limited to half the usual amount of its telekinetic powers.</t>
+  </si>
+  <si>
+    <t>A theory exists that this Pokémon was a young boy who couldn’t control his psychic powers and ended up transformed into this Pokémon.</t>
+  </si>
+  <si>
+    <t>Kadabra’s presence infests televisions and monitors with creepy shadows that bring bad luck.</t>
+  </si>
+  <si>
+    <t>It stares at a silver spoon to amplify its psychic powers before it lets loose. Apparently, gold spoons are no good.</t>
+  </si>
+  <si>
+    <t>It possesses strong mental capabilities, but its psychic powers are halved when it’s not holding a silver spoon.</t>
+  </si>
+  <si>
+    <t>Many odd things happen if this Pokémon is close by. For example, it makes clocks run backward.</t>
+  </si>
+  <si>
+    <t>Using its psychic power, Kadabra levitates as it sleeps. It uses its springy tail as a pillow.</t>
+  </si>
+  <si>
+    <t>This Pokémon’s telekinesis is immensely powerful. To prepare for evolution, Kadabra stores up psychic energy in the star on its forehead.</t>
+  </si>
+  <si>
+    <t>When it uses its psychic power, it emits strong alpha waves that can ruin precision instruments.</t>
+  </si>
+  <si>
+    <t>There are rumors that a child with mystical powers became a Kadabra; however, this remains unverified. I suspect that the spoon Kadabra holds enhances its brain waves.</t>
+  </si>
+  <si>
+    <t>48.0 kg</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>Its brain can outperform a supercomputer. Its intelligence quotient is said to be 5,000.</t>
+  </si>
+  <si>
+    <t>A POKéMON that can memorize anything. It never forgets what it learns--that’s why this POKéMON is smart.</t>
+  </si>
+  <si>
+    <t>Closing both its eyes heightens all its other senses. This enables it to use its abilities to their extremes.</t>
+  </si>
+  <si>
+    <t>Its brain cells multiply continually until it dies. As a result, it remembers everything.</t>
+  </si>
+  <si>
+    <t>It has an IQ of 5000. It calculates many things in order to gain the edge in every battle.</t>
+  </si>
+  <si>
+    <t>ALAKAZAM’s brain continually grows, making its head far too heavy to support with its neck. This POKéMON holds its head up using its psychokinetic power instead.</t>
+  </si>
+  <si>
+    <t>ALAKAZAM’s brain continually grows, infinitely multiplying brain cells. This amazing brain gives this POKéMON an astoundingly high IQ of 5,000. It has a thorough memory of everything that has occurred in the world.</t>
+  </si>
+  <si>
+    <t>It does not like physical attacks very much. Instead, it freely uses extrasensory powers to defeat foes.</t>
+  </si>
+  <si>
+    <t>Its brain can outperform a supercomputer. Its IQ (intelligence quotient) is said to be around 5,000.</t>
+  </si>
+  <si>
+    <t>While it has strong psychic abilities and high intelligence, an ALAKAZAM’s muscles are very weak. It uses psychic power to move its body.</t>
+  </si>
+  <si>
+    <t>Its superb memory lets it recall everything it has experienced from birth. Its IQ exceeds 5,000.</t>
+  </si>
+  <si>
+    <t>Its highly developed brain is on par with a supercomputer. It can use all forms of psychic abilities.</t>
+  </si>
+  <si>
+    <t>The spoons clutched in its hands are said to have been created by its psychic powers.</t>
+  </si>
+  <si>
+    <t>Alakazam’s brain continually grows, making its head far too heavy to support with its neck. This Pokémon holds its head up using its psychokinetic power instead.</t>
+  </si>
+  <si>
+    <t>Alakazam’s brain continually grows, infinitely multiplying brain cells. This amazing brain gives this Pokémon an astoundingly high IQ of 5,000. It has a thorough memory of everything that has occurred in the world.</t>
+  </si>
+  <si>
+    <t>It is said to have an IQ of approximately 5,000. Its overflowing psychokinetic powers cause headaches to anyone nearby.</t>
+  </si>
+  <si>
+    <t>Alakazam uses its psychic powers to make the spoons it carries. Each spoon is an original that there’s only one of in the whole world.</t>
+  </si>
+  <si>
+    <t>If it trusts someone deeply, it will let them have one of its spoons. Anything you eat with that spoon is apparently delicious.</t>
+  </si>
+  <si>
+    <t>A Pokémon that can memorize anything. It never forgets what it learns—that’s why this Pokémon is smart.</t>
+  </si>
+  <si>
+    <t>Alakazam wields potent psychic powers. It’s said that this Pokémon used these powers to create the spoons it holds.</t>
+  </si>
+  <si>
+    <t>The longer Alakazam lives, the larger and heavier its head becomes. Our tests have shown that the strength of its psychic powers correlates positively to the weight of its head.</t>
+  </si>
+  <si>
+    <t>As a result of Mega Evolution, its power has been entirely converted into psychic energy, and it has lost all strength in its muscles.</t>
+  </si>
+  <si>
+    <t>Its hidden psychic power has been unleashed. A glance at someone gives it knowledge of the course of that person’s life, from birth to death.</t>
+  </si>
+  <si>
+    <t>It sends out psychic power from the red organ on its forehead to foresee its opponents’ every move.</t>
+  </si>
+  <si>
+    <t>Having traded away its muscles, Alakazam’s true power has been unleashed. With its psychic powers, it can foresee all things.</t>
+  </si>
+  <si>
+    <t>It’s adept at precognition. When attacks completely miss Alakazam, that’s because it’s seeing the future.</t>
+  </si>
+  <si>
+    <t>Superpower Pokémon</t>
+  </si>
+  <si>
+    <t>Guts
+No guard
+Steadfast</t>
+  </si>
+  <si>
+    <t>70.5 kg</t>
+  </si>
+  <si>
+    <t>130.0 kg</t>
   </si>
 </sst>
 </file>
@@ -12566,8 +13452,8 @@
   <dimension ref="A1:ATT1216"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AST1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="ATS2" sqref="ATS2"/>
+      <pane xSplit="1" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CM1" sqref="CM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53664,6 +54550,60 @@
       <c r="BU13" s="4" t="s">
         <v>3601</v>
       </c>
+      <c r="BV13" s="4" t="s">
+        <v>3733</v>
+      </c>
+      <c r="BW13" s="4" t="s">
+        <v>3733</v>
+      </c>
+      <c r="BX13" s="4" t="s">
+        <v>3787</v>
+      </c>
+      <c r="BY13" s="4" t="s">
+        <v>3787</v>
+      </c>
+      <c r="BZ13" s="4" t="s">
+        <v>3825</v>
+      </c>
+      <c r="CA13" s="4" t="s">
+        <v>3829</v>
+      </c>
+      <c r="CB13" s="4" t="s">
+        <v>3853</v>
+      </c>
+      <c r="CC13" s="4" t="s">
+        <v>3853</v>
+      </c>
+      <c r="CD13" s="4" t="s">
+        <v>3877</v>
+      </c>
+      <c r="CE13" s="4" t="s">
+        <v>3877</v>
+      </c>
+      <c r="CF13" s="4" t="s">
+        <v>3877</v>
+      </c>
+      <c r="CG13" s="4" t="s">
+        <v>3937</v>
+      </c>
+      <c r="CH13" s="4" t="s">
+        <v>3937</v>
+      </c>
+      <c r="CI13" s="4" t="s">
+        <v>3937</v>
+      </c>
+      <c r="CJ13" s="4" t="s">
+        <v>3937</v>
+      </c>
+      <c r="CK13" s="4" t="s">
+        <v>4019</v>
+      </c>
+      <c r="CL13" s="4" t="s">
+        <v>4019</v>
+      </c>
+      <c r="CM13" s="4" t="s">
+        <v>4019</v>
+      </c>
     </row>
     <row r="14" spans="1:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -53885,6 +54825,60 @@
       <c r="BU14" s="10" t="s">
         <v>2564</v>
       </c>
+      <c r="BV14" s="10" t="s">
+        <v>2982</v>
+      </c>
+      <c r="BW14" s="10" t="s">
+        <v>2579</v>
+      </c>
+      <c r="BX14" s="10" t="s">
+        <v>3788</v>
+      </c>
+      <c r="BY14" s="10" t="s">
+        <v>2499</v>
+      </c>
+      <c r="BZ14" s="10" t="s">
+        <v>2478</v>
+      </c>
+      <c r="CA14" s="10" t="s">
+        <v>2982</v>
+      </c>
+      <c r="CB14" s="10" t="s">
+        <v>3854</v>
+      </c>
+      <c r="CC14" s="10" t="s">
+        <v>2542</v>
+      </c>
+      <c r="CD14" s="10" t="s">
+        <v>2547</v>
+      </c>
+      <c r="CE14" s="10" t="s">
+        <v>2499</v>
+      </c>
+      <c r="CF14" s="10" t="s">
+        <v>3098</v>
+      </c>
+      <c r="CG14" s="10" t="s">
+        <v>3145</v>
+      </c>
+      <c r="CH14" s="10" t="s">
+        <v>3098</v>
+      </c>
+      <c r="CI14" s="10" t="s">
+        <v>2809</v>
+      </c>
+      <c r="CJ14" s="10" t="s">
+        <v>2897</v>
+      </c>
+      <c r="CK14" s="10" t="s">
+        <v>2982</v>
+      </c>
+      <c r="CL14" s="10" t="s">
+        <v>2809</v>
+      </c>
+      <c r="CM14" s="10" t="s">
+        <v>2641</v>
+      </c>
     </row>
     <row r="15" spans="1:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -54106,6 +55100,60 @@
       <c r="BU15" t="s">
         <v>3603</v>
       </c>
+      <c r="BV15" t="s">
+        <v>3734</v>
+      </c>
+      <c r="BW15" t="s">
+        <v>3761</v>
+      </c>
+      <c r="BX15" t="s">
+        <v>3789</v>
+      </c>
+      <c r="BY15" t="s">
+        <v>2707</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>2565</v>
+      </c>
+      <c r="CA15" t="s">
+        <v>3830</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>3855</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>3856</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>3878</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>3095</v>
+      </c>
+      <c r="CF15" t="s">
+        <v>3917</v>
+      </c>
+      <c r="CG15" t="s">
+        <v>3146</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>3965</v>
+      </c>
+      <c r="CI15" t="s">
+        <v>3991</v>
+      </c>
+      <c r="CJ15" t="s">
+        <v>3991</v>
+      </c>
+      <c r="CK15" t="s">
+        <v>3146</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>4021</v>
+      </c>
+      <c r="CM15" t="s">
+        <v>4022</v>
+      </c>
       <c r="ATO15" s="1"/>
     </row>
     <row r="16" spans="1:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -54325,6 +55373,60 @@
       </c>
       <c r="BU16" s="2" t="s">
         <v>3604</v>
+      </c>
+      <c r="BV16" s="2" t="s">
+        <v>3735</v>
+      </c>
+      <c r="BW16" s="2" t="s">
+        <v>3735</v>
+      </c>
+      <c r="BX16" s="2" t="s">
+        <v>3790</v>
+      </c>
+      <c r="BY16" s="2" t="s">
+        <v>3790</v>
+      </c>
+      <c r="BZ16" s="2" t="s">
+        <v>3826</v>
+      </c>
+      <c r="CA16" s="2" t="s">
+        <v>3831</v>
+      </c>
+      <c r="CB16" s="2" t="s">
+        <v>3826</v>
+      </c>
+      <c r="CC16" s="2" t="s">
+        <v>3831</v>
+      </c>
+      <c r="CD16" s="2" t="s">
+        <v>3879</v>
+      </c>
+      <c r="CE16" s="2" t="s">
+        <v>3879</v>
+      </c>
+      <c r="CF16" s="2" t="s">
+        <v>3879</v>
+      </c>
+      <c r="CG16" s="2" t="s">
+        <v>3938</v>
+      </c>
+      <c r="CH16" s="2" t="s">
+        <v>3938</v>
+      </c>
+      <c r="CI16" s="2" t="s">
+        <v>3938</v>
+      </c>
+      <c r="CJ16" s="2" t="s">
+        <v>3992</v>
+      </c>
+      <c r="CK16" s="2" t="s">
+        <v>4020</v>
+      </c>
+      <c r="CL16" s="2" t="s">
+        <v>4020</v>
+      </c>
+      <c r="CM16" s="2" t="s">
+        <v>4020</v>
       </c>
       <c r="ATP16" s="2"/>
       <c r="ATQ16" s="2"/>
@@ -54332,7 +55434,7 @@
       <c r="ATS16" s="2"/>
       <c r="ATT16" s="2"/>
     </row>
-    <row r="17" spans="1:73 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:91 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2457</v>
       </c>
@@ -54551,6 +55653,60 @@
       </c>
       <c r="BU17" s="2" t="s">
         <v>2662</v>
+      </c>
+      <c r="BV17" s="2" t="s">
+        <v>2662</v>
+      </c>
+      <c r="BW17" s="2" t="s">
+        <v>2662</v>
+      </c>
+      <c r="BX17" s="2" t="s">
+        <v>2662</v>
+      </c>
+      <c r="BY17" s="2" t="s">
+        <v>2662</v>
+      </c>
+      <c r="BZ17" s="2" t="s">
+        <v>3827</v>
+      </c>
+      <c r="CA17" s="2" t="s">
+        <v>3827</v>
+      </c>
+      <c r="CB17" s="2" t="s">
+        <v>3827</v>
+      </c>
+      <c r="CC17" s="2" t="s">
+        <v>3827</v>
+      </c>
+      <c r="CD17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CE17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CF17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CG17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CH17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CI17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CJ17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CK17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CL17" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="CM17" s="2" t="s">
+        <v>2481</v>
       </c>
       <c r="ATO17" s="1"/>
       <c r="ATQ17" s="2"/>
@@ -54558,7 +55714,7 @@
       <c r="ATS17" s="2"/>
       <c r="ATT17" s="2"/>
     </row>
-    <row r="18" spans="1:73 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:91 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>2458</v>
       </c>
@@ -54772,6 +55928,60 @@
       </c>
       <c r="BU18" s="2" t="s">
         <v>2832</v>
+      </c>
+      <c r="BV18" s="2" t="s">
+        <v>3736</v>
+      </c>
+      <c r="BW18" s="2" t="s">
+        <v>3736</v>
+      </c>
+      <c r="BX18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="BY18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="BZ18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="CA18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="CB18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="CC18" s="2" t="s">
+        <v>2832</v>
+      </c>
+      <c r="CD18" s="2" t="s">
+        <v>3880</v>
+      </c>
+      <c r="CE18" s="2" t="s">
+        <v>3880</v>
+      </c>
+      <c r="CF18" s="2" t="s">
+        <v>3880</v>
+      </c>
+      <c r="CG18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CH18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CI18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CJ18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CK18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CL18" s="2" t="s">
+        <v>3939</v>
+      </c>
+      <c r="CM18" s="2" t="s">
+        <v>3939</v>
       </c>
       <c r="ATO18" s="1"/>
       <c r="ATP18" s="2"/>
@@ -54780,7 +55990,7 @@
       <c r="ATS18" s="2"/>
       <c r="ATT18" s="2"/>
     </row>
-    <row r="19" spans="1:73 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:91 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2459</v>
       </c>
@@ -54999,6 +56209,60 @@
       </c>
       <c r="BU19" s="2" t="s">
         <v>2779</v>
+      </c>
+      <c r="BV19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="BW19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="BX19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="BY19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="BZ19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CA19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CB19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CC19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CD19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="CE19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="CF19" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="CG19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CH19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CI19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CJ19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CK19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CL19" s="2" t="s">
+        <v>3828</v>
+      </c>
+      <c r="CM19" s="2" t="s">
+        <v>3828</v>
       </c>
       <c r="ATO19" s="1"/>
       <c r="ATP19" s="2"/>
@@ -55007,7 +56271,7 @@
       <c r="ATS19" s="2"/>
       <c r="ATT19" s="2"/>
     </row>
-    <row r="20" spans="1:73 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:91 1211:1216" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>2460</v>
       </c>
@@ -55227,9 +56491,63 @@
       <c r="BU20">
         <v>20</v>
       </c>
+      <c r="BV20">
+        <v>20</v>
+      </c>
+      <c r="BW20">
+        <v>20</v>
+      </c>
+      <c r="BX20">
+        <v>20</v>
+      </c>
+      <c r="BY20">
+        <v>20</v>
+      </c>
+      <c r="BZ20">
+        <v>20</v>
+      </c>
+      <c r="CA20">
+        <v>20</v>
+      </c>
+      <c r="CB20">
+        <v>20</v>
+      </c>
+      <c r="CC20">
+        <v>20</v>
+      </c>
+      <c r="CD20">
+        <v>20</v>
+      </c>
+      <c r="CE20">
+        <v>20</v>
+      </c>
+      <c r="CF20">
+        <v>20</v>
+      </c>
+      <c r="CG20">
+        <v>20</v>
+      </c>
+      <c r="CH20">
+        <v>20</v>
+      </c>
+      <c r="CI20">
+        <v>20</v>
+      </c>
+      <c r="CJ20">
+        <v>20</v>
+      </c>
+      <c r="CK20">
+        <v>20</v>
+      </c>
+      <c r="CL20">
+        <v>20</v>
+      </c>
+      <c r="CM20">
+        <v>20</v>
+      </c>
       <c r="ATO20" s="1"/>
     </row>
-    <row r="21" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>2497</v>
       </c>
@@ -55347,12 +56665,42 @@
       <c r="BS21" s="2" t="s">
         <v>3570</v>
       </c>
+      <c r="BV21" s="2" t="s">
+        <v>3737</v>
+      </c>
+      <c r="BX21" s="2" t="s">
+        <v>3570</v>
+      </c>
+      <c r="BZ21" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="CA21" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="CD21" s="2" t="s">
+        <v>3881</v>
+      </c>
+      <c r="CE21" s="2" t="s">
+        <v>3882</v>
+      </c>
+      <c r="CG21" s="2" t="s">
+        <v>2498</v>
+      </c>
+      <c r="CH21" s="2" t="s">
+        <v>3940</v>
+      </c>
+      <c r="CK21" s="2" t="s">
+        <v>3570</v>
+      </c>
+      <c r="CL21" s="2" t="s">
+        <v>3940</v>
+      </c>
       <c r="ATP21" s="2"/>
       <c r="ATQ21" s="2"/>
       <c r="ATS21" s="2"/>
       <c r="ATT21" s="2"/>
     </row>
-    <row r="22" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>2441</v>
       </c>
@@ -55522,6 +56870,42 @@
       </c>
       <c r="BT22" s="4" t="s">
         <v>3605</v>
+      </c>
+      <c r="BV22" s="4" t="s">
+        <v>3738</v>
+      </c>
+      <c r="BW22" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="BX22" s="4" t="s">
+        <v>3791</v>
+      </c>
+      <c r="BY22" s="4" t="s">
+        <v>3809</v>
+      </c>
+      <c r="BZ22" s="4" t="s">
+        <v>3832</v>
+      </c>
+      <c r="CB22" s="4" t="s">
+        <v>3857</v>
+      </c>
+      <c r="CD22" s="4" t="s">
+        <v>3883</v>
+      </c>
+      <c r="CE22" s="4" t="s">
+        <v>3900</v>
+      </c>
+      <c r="CF22" s="4" t="s">
+        <v>3918</v>
+      </c>
+      <c r="CG22" s="4" t="s">
+        <v>3941</v>
+      </c>
+      <c r="CH22" s="4" t="s">
+        <v>3966</v>
+      </c>
+      <c r="CI22" s="4" t="s">
+        <v>3993</v>
       </c>
       <c r="ATP22" s="8"/>
       <c r="ATQ22" s="8"/>
@@ -55529,7 +56913,7 @@
       <c r="ATS22" s="6"/>
       <c r="ATT22" s="3"/>
     </row>
-    <row r="23" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>2461</v>
       </c>
@@ -55699,6 +57083,42 @@
       </c>
       <c r="BT23" s="4" t="s">
         <v>3606</v>
+      </c>
+      <c r="BV23" s="4" t="s">
+        <v>3739</v>
+      </c>
+      <c r="BW23" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="BX23" s="4" t="s">
+        <v>3792</v>
+      </c>
+      <c r="BY23" s="4" t="s">
+        <v>3810</v>
+      </c>
+      <c r="BZ23" s="4" t="s">
+        <v>3833</v>
+      </c>
+      <c r="CB23" s="4" t="s">
+        <v>3858</v>
+      </c>
+      <c r="CD23" s="4" t="s">
+        <v>3884</v>
+      </c>
+      <c r="CE23" s="4" t="s">
+        <v>3901</v>
+      </c>
+      <c r="CF23" s="4" t="s">
+        <v>3919</v>
+      </c>
+      <c r="CG23" s="4" t="s">
+        <v>3942</v>
+      </c>
+      <c r="CH23" s="4" t="s">
+        <v>3967</v>
+      </c>
+      <c r="CI23" s="4" t="s">
+        <v>3994</v>
       </c>
       <c r="ATO23" s="1"/>
       <c r="ATP23" s="8"/>
@@ -55707,7 +57127,7 @@
       <c r="ATS23" s="6"/>
       <c r="ATT23" s="3"/>
     </row>
-    <row r="24" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>2462</v>
       </c>
@@ -55877,6 +57297,42 @@
       </c>
       <c r="BT24" s="4" t="s">
         <v>3607</v>
+      </c>
+      <c r="BV24" s="4" t="s">
+        <v>3740</v>
+      </c>
+      <c r="BW24" s="4" t="s">
+        <v>3764</v>
+      </c>
+      <c r="BX24" s="4" t="s">
+        <v>3793</v>
+      </c>
+      <c r="BY24" s="4" t="s">
+        <v>3811</v>
+      </c>
+      <c r="BZ24" s="4" t="s">
+        <v>3834</v>
+      </c>
+      <c r="CB24" s="4" t="s">
+        <v>3858</v>
+      </c>
+      <c r="CD24" s="4" t="s">
+        <v>3885</v>
+      </c>
+      <c r="CE24" s="4" t="s">
+        <v>3902</v>
+      </c>
+      <c r="CF24" s="4" t="s">
+        <v>3920</v>
+      </c>
+      <c r="CG24" s="4" t="s">
+        <v>3943</v>
+      </c>
+      <c r="CH24" s="4" t="s">
+        <v>3968</v>
+      </c>
+      <c r="CI24" s="4" t="s">
+        <v>3995</v>
       </c>
       <c r="ATO24" s="1"/>
       <c r="ATP24" s="8"/>
@@ -55885,7 +57341,7 @@
       <c r="ATS24" s="6"/>
       <c r="ATT24" s="3"/>
     </row>
-    <row r="25" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>2463</v>
       </c>
@@ -56055,6 +57511,42 @@
       </c>
       <c r="BT25" s="4" t="s">
         <v>3608</v>
+      </c>
+      <c r="BV25" s="4" t="s">
+        <v>3741</v>
+      </c>
+      <c r="BW25" s="4" t="s">
+        <v>3765</v>
+      </c>
+      <c r="BX25" s="4" t="s">
+        <v>3794</v>
+      </c>
+      <c r="BY25" s="4" t="s">
+        <v>3812</v>
+      </c>
+      <c r="BZ25" s="4" t="s">
+        <v>3835</v>
+      </c>
+      <c r="CB25" s="4" t="s">
+        <v>3859</v>
+      </c>
+      <c r="CD25" s="4" t="s">
+        <v>3886</v>
+      </c>
+      <c r="CE25" s="4" t="s">
+        <v>3903</v>
+      </c>
+      <c r="CF25" s="4" t="s">
+        <v>3921</v>
+      </c>
+      <c r="CG25" s="4" t="s">
+        <v>3944</v>
+      </c>
+      <c r="CH25" s="4" t="s">
+        <v>3969</v>
+      </c>
+      <c r="CI25" s="4" t="s">
+        <v>3996</v>
       </c>
       <c r="ATO25" s="1"/>
       <c r="ATP25" s="8"/>
@@ -56063,7 +57555,7 @@
       <c r="ATS25" s="6"/>
       <c r="ATT25" s="3"/>
     </row>
-    <row r="26" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>2464</v>
       </c>
@@ -56233,6 +57725,42 @@
       </c>
       <c r="BT26" s="4" t="s">
         <v>3609</v>
+      </c>
+      <c r="BV26" s="4" t="s">
+        <v>3742</v>
+      </c>
+      <c r="BW26" s="4" t="s">
+        <v>3766</v>
+      </c>
+      <c r="BX26" s="4" t="s">
+        <v>3795</v>
+      </c>
+      <c r="BY26" s="4" t="s">
+        <v>3813</v>
+      </c>
+      <c r="BZ26" s="4" t="s">
+        <v>3836</v>
+      </c>
+      <c r="CB26" s="4" t="s">
+        <v>3860</v>
+      </c>
+      <c r="CD26" s="4" t="s">
+        <v>3887</v>
+      </c>
+      <c r="CE26" s="4" t="s">
+        <v>3904</v>
+      </c>
+      <c r="CF26" s="4" t="s">
+        <v>3922</v>
+      </c>
+      <c r="CG26" s="4" t="s">
+        <v>3945</v>
+      </c>
+      <c r="CH26" s="4" t="s">
+        <v>3970</v>
+      </c>
+      <c r="CI26" s="4" t="s">
+        <v>3997</v>
       </c>
       <c r="ATO26" s="1"/>
       <c r="ATP26" s="8"/>
@@ -56241,7 +57769,7 @@
       <c r="ATS26" s="7"/>
       <c r="ATT26" s="3"/>
     </row>
-    <row r="27" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>2509</v>
       </c>
@@ -56411,6 +57939,42 @@
       </c>
       <c r="BT27" s="4" t="s">
         <v>3610</v>
+      </c>
+      <c r="BV27" s="4" t="s">
+        <v>3743</v>
+      </c>
+      <c r="BW27" s="4" t="s">
+        <v>3767</v>
+      </c>
+      <c r="BX27" s="4" t="s">
+        <v>3796</v>
+      </c>
+      <c r="BY27" s="4" t="s">
+        <v>3814</v>
+      </c>
+      <c r="BZ27" s="4" t="s">
+        <v>3837</v>
+      </c>
+      <c r="CB27" s="4" t="s">
+        <v>3861</v>
+      </c>
+      <c r="CD27" s="4" t="s">
+        <v>3888</v>
+      </c>
+      <c r="CE27" s="4" t="s">
+        <v>3905</v>
+      </c>
+      <c r="CF27" s="4" t="s">
+        <v>3923</v>
+      </c>
+      <c r="CG27" s="4" t="s">
+        <v>3946</v>
+      </c>
+      <c r="CH27" s="4" t="s">
+        <v>3971</v>
+      </c>
+      <c r="CI27" s="4" t="s">
+        <v>3998</v>
       </c>
       <c r="ATO27" s="1"/>
       <c r="ATP27" s="8"/>
@@ -56419,7 +57983,7 @@
       <c r="ATS27" s="6"/>
       <c r="ATT27" s="3"/>
     </row>
-    <row r="28" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>2510</v>
       </c>
@@ -56589,6 +58153,42 @@
       </c>
       <c r="BT28" s="4" t="s">
         <v>3610</v>
+      </c>
+      <c r="BV28" s="4" t="s">
+        <v>3744</v>
+      </c>
+      <c r="BW28" s="4" t="s">
+        <v>3768</v>
+      </c>
+      <c r="BX28" s="4" t="s">
+        <v>3796</v>
+      </c>
+      <c r="BY28" s="4" t="s">
+        <v>3814</v>
+      </c>
+      <c r="BZ28" s="4" t="s">
+        <v>3837</v>
+      </c>
+      <c r="CB28" s="4" t="s">
+        <v>3861</v>
+      </c>
+      <c r="CD28" s="4" t="s">
+        <v>3888</v>
+      </c>
+      <c r="CE28" s="4" t="s">
+        <v>3905</v>
+      </c>
+      <c r="CF28" s="4" t="s">
+        <v>3923</v>
+      </c>
+      <c r="CG28" s="4" t="s">
+        <v>3947</v>
+      </c>
+      <c r="CH28" s="4" t="s">
+        <v>3972</v>
+      </c>
+      <c r="CI28" s="4" t="s">
+        <v>3999</v>
       </c>
       <c r="ATP28" s="8"/>
       <c r="ATQ28" s="8"/>
@@ -56596,7 +58196,7 @@
       <c r="ATS28" s="7"/>
       <c r="ATT28" s="3"/>
     </row>
-    <row r="29" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>2465</v>
       </c>
@@ -56766,6 +58366,42 @@
       </c>
       <c r="BT29" s="4" t="s">
         <v>3611</v>
+      </c>
+      <c r="BV29" s="4" t="s">
+        <v>3745</v>
+      </c>
+      <c r="BW29" s="4" t="s">
+        <v>3769</v>
+      </c>
+      <c r="BX29" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="BY29" s="4" t="s">
+        <v>3815</v>
+      </c>
+      <c r="BZ29" s="4" t="s">
+        <v>3838</v>
+      </c>
+      <c r="CB29" s="4" t="s">
+        <v>3862</v>
+      </c>
+      <c r="CD29" s="4" t="s">
+        <v>3889</v>
+      </c>
+      <c r="CE29" s="10" t="s">
+        <v>3906</v>
+      </c>
+      <c r="CF29" s="4" t="s">
+        <v>3924</v>
+      </c>
+      <c r="CG29" s="4" t="s">
+        <v>3948</v>
+      </c>
+      <c r="CH29" s="4" t="s">
+        <v>3973</v>
+      </c>
+      <c r="CI29" s="4" t="s">
+        <v>4000</v>
       </c>
       <c r="ATO29" s="1"/>
       <c r="ATP29" s="9"/>
@@ -56774,7 +58410,7 @@
       <c r="ATS29" s="6"/>
       <c r="ATT29" s="3"/>
     </row>
-    <row r="30" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>2466</v>
       </c>
@@ -56944,6 +58580,42 @@
       </c>
       <c r="BT30" s="4" t="s">
         <v>3605</v>
+      </c>
+      <c r="BV30" s="4" t="s">
+        <v>3738</v>
+      </c>
+      <c r="BW30" s="4" t="s">
+        <v>3770</v>
+      </c>
+      <c r="BX30" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="BY30" s="4" t="s">
+        <v>3816</v>
+      </c>
+      <c r="BZ30" s="4" t="s">
+        <v>3839</v>
+      </c>
+      <c r="CB30" s="4" t="s">
+        <v>3863</v>
+      </c>
+      <c r="CD30" s="4" t="s">
+        <v>3890</v>
+      </c>
+      <c r="CE30" s="4" t="s">
+        <v>3907</v>
+      </c>
+      <c r="CF30" s="4" t="s">
+        <v>3925</v>
+      </c>
+      <c r="CG30" s="4" t="s">
+        <v>3949</v>
+      </c>
+      <c r="CH30" s="4" t="s">
+        <v>3974</v>
+      </c>
+      <c r="CI30" s="4" t="s">
+        <v>4001</v>
       </c>
       <c r="ATP30" s="8"/>
       <c r="ATQ30" s="8"/>
@@ -56951,7 +58623,7 @@
       <c r="ATS30" s="6"/>
       <c r="ATT30" s="3"/>
     </row>
-    <row r="31" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>2511</v>
       </c>
@@ -57121,6 +58793,42 @@
       </c>
       <c r="BT31" s="4" t="s">
         <v>3612</v>
+      </c>
+      <c r="BV31" s="4" t="s">
+        <v>3746</v>
+      </c>
+      <c r="BW31" s="4" t="s">
+        <v>3771</v>
+      </c>
+      <c r="BX31" s="4" t="s">
+        <v>3799</v>
+      </c>
+      <c r="BY31" s="4" t="s">
+        <v>3817</v>
+      </c>
+      <c r="BZ31" s="4" t="s">
+        <v>3840</v>
+      </c>
+      <c r="CB31" s="4" t="s">
+        <v>3864</v>
+      </c>
+      <c r="CD31" s="4" t="s">
+        <v>3891</v>
+      </c>
+      <c r="CE31" s="4" t="s">
+        <v>3908</v>
+      </c>
+      <c r="CF31" s="4" t="s">
+        <v>3926</v>
+      </c>
+      <c r="CG31" s="4" t="s">
+        <v>3950</v>
+      </c>
+      <c r="CH31" s="4" t="s">
+        <v>3975</v>
+      </c>
+      <c r="CI31" s="4" t="s">
+        <v>4002</v>
       </c>
       <c r="ATP31" s="8"/>
       <c r="ATQ31" s="8"/>
@@ -57128,7 +58836,7 @@
       <c r="ATS31" s="6"/>
       <c r="ATT31" s="3"/>
     </row>
-    <row r="32" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:91 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>2512</v>
       </c>
@@ -57298,6 +59006,42 @@
       </c>
       <c r="BT32" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV32" s="4" t="s">
+        <v>3747</v>
+      </c>
+      <c r="BW32" s="4" t="s">
+        <v>3772</v>
+      </c>
+      <c r="BX32" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY32" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ32" s="4" t="s">
+        <v>3841</v>
+      </c>
+      <c r="CB32" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD32" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE32" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF32" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG32" s="4" t="s">
+        <v>3951</v>
+      </c>
+      <c r="CH32" s="4" t="s">
+        <v>3976</v>
+      </c>
+      <c r="CI32" s="4" t="s">
+        <v>4003</v>
       </c>
       <c r="ATO32" s="1"/>
       <c r="ATP32" s="8"/>
@@ -57306,7 +59050,7 @@
       <c r="ATS32" s="7"/>
       <c r="ATT32" s="3"/>
     </row>
-    <row r="33" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>2513</v>
       </c>
@@ -57476,6 +59220,42 @@
       </c>
       <c r="BT33" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV33" s="4" t="s">
+        <v>3748</v>
+      </c>
+      <c r="BW33" s="4" t="s">
+        <v>3773</v>
+      </c>
+      <c r="BX33" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY33" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ33" s="4" t="s">
+        <v>3841</v>
+      </c>
+      <c r="CB33" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD33" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE33" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF33" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG33" s="4" t="s">
+        <v>3952</v>
+      </c>
+      <c r="CH33" s="4" t="s">
+        <v>3977</v>
+      </c>
+      <c r="CI33" s="4" t="s">
+        <v>4004</v>
       </c>
       <c r="ATP33" s="8"/>
       <c r="ATQ33" s="8"/>
@@ -57483,7 +59263,7 @@
       <c r="ATS33" s="7"/>
       <c r="ATT33" s="3"/>
     </row>
-    <row r="34" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>2514</v>
       </c>
@@ -57653,6 +59433,42 @@
       </c>
       <c r="BT34" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV34" s="4" t="s">
+        <v>3749</v>
+      </c>
+      <c r="BW34" s="4" t="s">
+        <v>3774</v>
+      </c>
+      <c r="BX34" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY34" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ34" s="4" t="s">
+        <v>3841</v>
+      </c>
+      <c r="CB34" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD34" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE34" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF34" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG34" s="4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="CH34" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="CI34" s="4" t="s">
+        <v>4005</v>
       </c>
       <c r="ATP34" s="8"/>
       <c r="ATQ34" s="8"/>
@@ -57660,7 +59476,7 @@
       <c r="ATS34" s="7"/>
       <c r="ATT34" s="3"/>
     </row>
-    <row r="35" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>2467</v>
       </c>
@@ -57830,6 +59646,42 @@
       </c>
       <c r="BT35" s="4" t="s">
         <v>3607</v>
+      </c>
+      <c r="BV35" s="4" t="s">
+        <v>3740</v>
+      </c>
+      <c r="BW35" s="4" t="s">
+        <v>3764</v>
+      </c>
+      <c r="BX35" s="4" t="s">
+        <v>3793</v>
+      </c>
+      <c r="BY35" s="4" t="s">
+        <v>3811</v>
+      </c>
+      <c r="BZ35" s="4" t="s">
+        <v>3834</v>
+      </c>
+      <c r="CB35" s="4" t="s">
+        <v>3866</v>
+      </c>
+      <c r="CD35" s="4" t="s">
+        <v>3885</v>
+      </c>
+      <c r="CE35" s="4" t="s">
+        <v>3902</v>
+      </c>
+      <c r="CF35" s="4" t="s">
+        <v>3920</v>
+      </c>
+      <c r="CG35" s="4" t="s">
+        <v>3954</v>
+      </c>
+      <c r="CH35" s="4" t="s">
+        <v>3968</v>
+      </c>
+      <c r="CI35" s="4" t="s">
+        <v>3995</v>
       </c>
       <c r="ATO35" s="1"/>
       <c r="ATP35" s="8"/>
@@ -57838,7 +59690,7 @@
       <c r="ATS35" s="7"/>
       <c r="ATT35" s="3"/>
     </row>
-    <row r="36" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>2468</v>
       </c>
@@ -58008,6 +59860,42 @@
       </c>
       <c r="BT36" s="4" t="s">
         <v>3608</v>
+      </c>
+      <c r="BV36" s="4" t="s">
+        <v>3741</v>
+      </c>
+      <c r="BW36" s="4" t="s">
+        <v>3765</v>
+      </c>
+      <c r="BX36" s="4" t="s">
+        <v>3794</v>
+      </c>
+      <c r="BY36" s="4" t="s">
+        <v>3812</v>
+      </c>
+      <c r="BZ36" s="4" t="s">
+        <v>3842</v>
+      </c>
+      <c r="CB36" s="4" t="s">
+        <v>3859</v>
+      </c>
+      <c r="CD36" s="4" t="s">
+        <v>3886</v>
+      </c>
+      <c r="CE36" s="4" t="s">
+        <v>3903</v>
+      </c>
+      <c r="CF36" s="4" t="s">
+        <v>3921</v>
+      </c>
+      <c r="CG36" s="4" t="s">
+        <v>3955</v>
+      </c>
+      <c r="CH36" s="4" t="s">
+        <v>3969</v>
+      </c>
+      <c r="CI36" s="4" t="s">
+        <v>3996</v>
       </c>
       <c r="ATO36" s="1"/>
       <c r="ATP36" s="8"/>
@@ -58016,7 +59904,7 @@
       <c r="ATS36" s="7"/>
       <c r="ATT36" s="4"/>
     </row>
-    <row r="37" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>2515</v>
       </c>
@@ -58186,6 +60074,42 @@
       </c>
       <c r="BT37" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV37" s="4" t="s">
+        <v>3749</v>
+      </c>
+      <c r="BW37" s="4" t="s">
+        <v>3774</v>
+      </c>
+      <c r="BX37" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY37" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ37" s="4" t="s">
+        <v>3841</v>
+      </c>
+      <c r="CB37" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD37" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE37" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF37" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG37" s="4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="CH37" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="CI37" s="4" t="s">
+        <v>4005</v>
       </c>
       <c r="ATO37" s="1"/>
       <c r="ATP37" s="8"/>
@@ -58194,7 +60118,7 @@
       <c r="ATS37" s="6"/>
       <c r="ATT37" s="3"/>
     </row>
-    <row r="38" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>2516</v>
       </c>
@@ -58364,6 +60288,42 @@
       </c>
       <c r="BT38" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV38" s="4" t="s">
+        <v>3749</v>
+      </c>
+      <c r="BW38" s="4" t="s">
+        <v>3774</v>
+      </c>
+      <c r="BX38" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY38" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ38" s="4" t="s">
+        <v>3841</v>
+      </c>
+      <c r="CB38" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD38" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE38" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF38" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG38" s="4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="CH38" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="CI38" s="4" t="s">
+        <v>4005</v>
       </c>
       <c r="ATP38" s="8"/>
       <c r="ATQ38" s="8"/>
@@ -58371,7 +60331,7 @@
       <c r="ATS38" s="7"/>
       <c r="ATT38" s="3"/>
     </row>
-    <row r="39" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>2517</v>
       </c>
@@ -58541,6 +60501,42 @@
       </c>
       <c r="BT39" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV39" s="4" t="s">
+        <v>3750</v>
+      </c>
+      <c r="BW39" s="4" t="s">
+        <v>3775</v>
+      </c>
+      <c r="BX39" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY39" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ39" s="4" t="s">
+        <v>3843</v>
+      </c>
+      <c r="CB39" s="4" t="s">
+        <v>3867</v>
+      </c>
+      <c r="CD39" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE39" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF39" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG39" s="4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="CH39" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="CI39" s="4" t="s">
+        <v>4005</v>
       </c>
       <c r="ATP39" s="8"/>
       <c r="ATQ39" s="8"/>
@@ -58548,7 +60544,7 @@
       <c r="ATS39" s="6"/>
       <c r="ATT39" s="3"/>
     </row>
-    <row r="40" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>2518</v>
       </c>
@@ -58718,6 +60714,42 @@
       </c>
       <c r="BT40" s="4" t="s">
         <v>3613</v>
+      </c>
+      <c r="BV40" s="4" t="s">
+        <v>3750</v>
+      </c>
+      <c r="BW40" s="4" t="s">
+        <v>3775</v>
+      </c>
+      <c r="BX40" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY40" s="4" t="s">
+        <v>3818</v>
+      </c>
+      <c r="BZ40" s="4" t="s">
+        <v>3843</v>
+      </c>
+      <c r="CB40" s="4" t="s">
+        <v>3867</v>
+      </c>
+      <c r="CD40" s="4" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE40" s="4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF40" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG40" s="4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="CH40" s="4" t="s">
+        <v>3978</v>
+      </c>
+      <c r="CI40" s="4" t="s">
+        <v>4005</v>
       </c>
       <c r="ATP40" s="8"/>
       <c r="ATQ40" s="8"/>
@@ -58725,7 +60757,7 @@
       <c r="ATS40" s="7"/>
       <c r="ATT40" s="3"/>
     </row>
-    <row r="41" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>2469</v>
       </c>
@@ -58895,6 +60927,42 @@
       </c>
       <c r="BT41" s="4" t="s">
         <v>3605</v>
+      </c>
+      <c r="BV41" s="4" t="s">
+        <v>3745</v>
+      </c>
+      <c r="BW41" s="4" t="s">
+        <v>3765</v>
+      </c>
+      <c r="BX41" s="4" t="s">
+        <v>3794</v>
+      </c>
+      <c r="BY41" s="4" t="s">
+        <v>3810</v>
+      </c>
+      <c r="BZ41" s="4" t="s">
+        <v>3838</v>
+      </c>
+      <c r="CB41" s="4" t="s">
+        <v>3868</v>
+      </c>
+      <c r="CD41" s="4" t="s">
+        <v>3889</v>
+      </c>
+      <c r="CE41" s="4" t="s">
+        <v>3907</v>
+      </c>
+      <c r="CF41" s="4" t="s">
+        <v>3927</v>
+      </c>
+      <c r="CG41" s="4" t="s">
+        <v>3948</v>
+      </c>
+      <c r="CH41" s="4" t="s">
+        <v>3979</v>
+      </c>
+      <c r="CI41" s="4" t="s">
+        <v>3996</v>
       </c>
       <c r="ATO41" s="1"/>
       <c r="ATP41" s="8"/>
@@ -58903,7 +60971,7 @@
       <c r="ATS41" s="6"/>
       <c r="ATT41" s="3"/>
     </row>
-    <row r="42" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>2470</v>
       </c>
@@ -59073,6 +61141,42 @@
       </c>
       <c r="BT42" s="4" t="s">
         <v>3608</v>
+      </c>
+      <c r="BV42" s="4" t="s">
+        <v>3740</v>
+      </c>
+      <c r="BW42" s="4" t="s">
+        <v>3769</v>
+      </c>
+      <c r="BX42" s="4" t="s">
+        <v>3800</v>
+      </c>
+      <c r="BY42" s="4" t="s">
+        <v>3815</v>
+      </c>
+      <c r="BZ42" s="4" t="s">
+        <v>3834</v>
+      </c>
+      <c r="CB42" s="4" t="s">
+        <v>3859</v>
+      </c>
+      <c r="CD42" s="4" t="s">
+        <v>3884</v>
+      </c>
+      <c r="CE42" s="4" t="s">
+        <v>3906</v>
+      </c>
+      <c r="CF42" s="4" t="s">
+        <v>3925</v>
+      </c>
+      <c r="CG42" s="4" t="s">
+        <v>3954</v>
+      </c>
+      <c r="CH42" s="4" t="s">
+        <v>3969</v>
+      </c>
+      <c r="CI42" s="4" t="s">
+        <v>4001</v>
       </c>
       <c r="ATO42" s="1"/>
       <c r="ATP42" s="8"/>
@@ -59081,7 +61185,7 @@
       <c r="ATS42" s="7"/>
       <c r="ATT42" s="3"/>
     </row>
-    <row r="43" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>2519</v>
       </c>
@@ -59251,6 +61355,42 @@
       </c>
       <c r="BT43" s="4" t="s">
         <v>3614</v>
+      </c>
+      <c r="BV43" s="4" t="s">
+        <v>3751</v>
+      </c>
+      <c r="BW43" s="4" t="s">
+        <v>3776</v>
+      </c>
+      <c r="BX43" s="4" t="s">
+        <v>3801</v>
+      </c>
+      <c r="BY43" s="4" t="s">
+        <v>3819</v>
+      </c>
+      <c r="BZ43" s="4" t="s">
+        <v>3844</v>
+      </c>
+      <c r="CB43" s="4" t="s">
+        <v>3869</v>
+      </c>
+      <c r="CD43" s="4" t="s">
+        <v>3893</v>
+      </c>
+      <c r="CE43" s="4" t="s">
+        <v>3910</v>
+      </c>
+      <c r="CF43" s="4" t="s">
+        <v>3928</v>
+      </c>
+      <c r="CG43" s="4" t="s">
+        <v>3956</v>
+      </c>
+      <c r="CH43" s="4" t="s">
+        <v>3980</v>
+      </c>
+      <c r="CI43" s="4" t="s">
+        <v>4006</v>
       </c>
       <c r="ATO43" s="1"/>
       <c r="ATP43" s="8"/>
@@ -59259,7 +61399,7 @@
       <c r="ATS43" s="7"/>
       <c r="ATT43" s="3"/>
     </row>
-    <row r="44" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>2520</v>
       </c>
@@ -59429,6 +61569,42 @@
       </c>
       <c r="BT44" s="4" t="s">
         <v>3614</v>
+      </c>
+      <c r="BV44" s="4" t="s">
+        <v>3752</v>
+      </c>
+      <c r="BW44" s="4" t="s">
+        <v>3777</v>
+      </c>
+      <c r="BX44" s="4" t="s">
+        <v>3801</v>
+      </c>
+      <c r="BY44" s="4" t="s">
+        <v>3819</v>
+      </c>
+      <c r="BZ44" s="4" t="s">
+        <v>3844</v>
+      </c>
+      <c r="CB44" s="4" t="s">
+        <v>3869</v>
+      </c>
+      <c r="CD44" s="4" t="s">
+        <v>3893</v>
+      </c>
+      <c r="CE44" s="4" t="s">
+        <v>3910</v>
+      </c>
+      <c r="CF44" s="4" t="s">
+        <v>3928</v>
+      </c>
+      <c r="CG44" s="4" t="s">
+        <v>3957</v>
+      </c>
+      <c r="CH44" s="4" t="s">
+        <v>3981</v>
+      </c>
+      <c r="CI44" s="4" t="s">
+        <v>4007</v>
       </c>
       <c r="ATP44" s="8"/>
       <c r="ATQ44" s="8"/>
@@ -59436,7 +61612,7 @@
       <c r="ATS44" s="6"/>
       <c r="ATT44" s="3"/>
     </row>
-    <row r="45" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>2676</v>
       </c>
@@ -59561,8 +61737,47 @@
       <c r="BU45" s="4" t="s">
         <v>3623</v>
       </c>
-    </row>
-    <row r="46" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BV45" s="4" t="s">
+        <v>3753</v>
+      </c>
+      <c r="BW45" s="4" t="s">
+        <v>3778</v>
+      </c>
+      <c r="BX45" s="4" t="s">
+        <v>3802</v>
+      </c>
+      <c r="BY45" s="4" t="s">
+        <v>3820</v>
+      </c>
+      <c r="BZ45" s="4" t="s">
+        <v>3845</v>
+      </c>
+      <c r="CB45" s="4" t="s">
+        <v>3870</v>
+      </c>
+      <c r="CD45" s="4" t="s">
+        <v>3894</v>
+      </c>
+      <c r="CE45" s="4" t="s">
+        <v>3911</v>
+      </c>
+      <c r="CF45" s="4" t="s">
+        <v>3929</v>
+      </c>
+      <c r="CG45" s="4" t="s">
+        <v>3958</v>
+      </c>
+      <c r="CH45" s="4" t="s">
+        <v>3982</v>
+      </c>
+      <c r="CI45" s="4" t="s">
+        <v>4008</v>
+      </c>
+      <c r="CJ45" s="4" t="s">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="46" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>2677</v>
       </c>
@@ -59674,8 +61889,45 @@
       <c r="BU46" s="4" t="s">
         <v>3624</v>
       </c>
-    </row>
-    <row r="47" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BV46" s="4" t="s">
+        <v>3754</v>
+      </c>
+      <c r="BW46" s="4" t="s">
+        <v>3779</v>
+      </c>
+      <c r="BX46" s="4" t="s">
+        <v>3803</v>
+      </c>
+      <c r="BY46" s="4" t="s">
+        <v>3821</v>
+      </c>
+      <c r="BZ46" s="4" t="s">
+        <v>3846</v>
+      </c>
+      <c r="CB46" s="4" t="s">
+        <v>3871</v>
+      </c>
+      <c r="CD46" s="4" t="s">
+        <v>3895</v>
+      </c>
+      <c r="CE46" s="4" t="s">
+        <v>3912</v>
+      </c>
+      <c r="CF46" s="4" t="s">
+        <v>3930</v>
+      </c>
+      <c r="CG46" s="4" t="s">
+        <v>3959</v>
+      </c>
+      <c r="CH46" s="4" t="s">
+        <v>3983</v>
+      </c>
+      <c r="CI46" s="10"/>
+      <c r="CJ46" s="4" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="47" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>2678</v>
       </c>
@@ -59793,8 +62045,47 @@
       <c r="BU47" s="4" t="s">
         <v>3625</v>
       </c>
-    </row>
-    <row r="48" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BV47" s="4" t="s">
+        <v>3755</v>
+      </c>
+      <c r="BW47" s="4" t="s">
+        <v>3780</v>
+      </c>
+      <c r="BX47" s="4" t="s">
+        <v>3804</v>
+      </c>
+      <c r="BY47" s="4" t="s">
+        <v>3822</v>
+      </c>
+      <c r="BZ47" s="4" t="s">
+        <v>3847</v>
+      </c>
+      <c r="CB47" s="4" t="s">
+        <v>3872</v>
+      </c>
+      <c r="CD47" s="4" t="s">
+        <v>3896</v>
+      </c>
+      <c r="CE47" s="4" t="s">
+        <v>3913</v>
+      </c>
+      <c r="CF47" s="4" t="s">
+        <v>3931</v>
+      </c>
+      <c r="CG47" s="4" t="s">
+        <v>3960</v>
+      </c>
+      <c r="CH47" s="4" t="s">
+        <v>3984</v>
+      </c>
+      <c r="CI47" s="4" t="s">
+        <v>4009</v>
+      </c>
+      <c r="CJ47" s="4" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="48" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>2679</v>
       </c>
@@ -59912,8 +62203,47 @@
       <c r="BU48" s="4" t="s">
         <v>3626</v>
       </c>
-    </row>
-    <row r="49" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BV48" s="4" t="s">
+        <v>3756</v>
+      </c>
+      <c r="BW48" s="4" t="s">
+        <v>3781</v>
+      </c>
+      <c r="BX48" s="4" t="s">
+        <v>3805</v>
+      </c>
+      <c r="BY48" s="4" t="s">
+        <v>3823</v>
+      </c>
+      <c r="BZ48" s="4" t="s">
+        <v>3848</v>
+      </c>
+      <c r="CB48" s="4" t="s">
+        <v>3873</v>
+      </c>
+      <c r="CD48" s="4" t="s">
+        <v>3897</v>
+      </c>
+      <c r="CE48" s="4" t="s">
+        <v>3914</v>
+      </c>
+      <c r="CF48" s="4" t="s">
+        <v>3932</v>
+      </c>
+      <c r="CG48" s="4" t="s">
+        <v>3961</v>
+      </c>
+      <c r="CH48" s="4" t="s">
+        <v>3985</v>
+      </c>
+      <c r="CI48" s="4" t="s">
+        <v>4010</v>
+      </c>
+      <c r="CJ48" s="4" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="49" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>2521</v>
       </c>
@@ -60124,6 +62454,45 @@
       </c>
       <c r="BU49" s="4" t="s">
         <v>3627</v>
+      </c>
+      <c r="BV49" s="4" t="s">
+        <v>3757</v>
+      </c>
+      <c r="BW49" s="4" t="s">
+        <v>3782</v>
+      </c>
+      <c r="BX49" s="4" t="s">
+        <v>3806</v>
+      </c>
+      <c r="BY49" s="4" t="s">
+        <v>3810</v>
+      </c>
+      <c r="BZ49" s="4" t="s">
+        <v>3849</v>
+      </c>
+      <c r="CB49" s="4" t="s">
+        <v>3874</v>
+      </c>
+      <c r="CD49" s="4" t="s">
+        <v>3884</v>
+      </c>
+      <c r="CE49" s="4" t="s">
+        <v>3901</v>
+      </c>
+      <c r="CF49" s="4" t="s">
+        <v>3933</v>
+      </c>
+      <c r="CG49" s="4" t="s">
+        <v>3942</v>
+      </c>
+      <c r="CH49" s="4" t="s">
+        <v>3986</v>
+      </c>
+      <c r="CI49" s="4" t="s">
+        <v>4011</v>
+      </c>
+      <c r="CJ49" s="11" t="s">
+        <v>4018</v>
       </c>
       <c r="ATO49" s="1"/>
       <c r="ATP49" s="9"/>
@@ -60132,7 +62501,7 @@
       <c r="ATS49" s="8"/>
       <c r="ATT49" s="3"/>
     </row>
-    <row r="50" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>2471</v>
       </c>
@@ -60303,6 +62672,36 @@
       <c r="BU50" s="4" t="s">
         <v>3628</v>
       </c>
+      <c r="BV50" s="4" t="s">
+        <v>3758</v>
+      </c>
+      <c r="BW50" s="4" t="s">
+        <v>3783</v>
+      </c>
+      <c r="BX50" s="10"/>
+      <c r="BY50" s="10"/>
+      <c r="BZ50" s="4" t="s">
+        <v>3834</v>
+      </c>
+      <c r="CB50" s="4" t="s">
+        <v>3867</v>
+      </c>
+      <c r="CD50" s="4" t="s">
+        <v>3898</v>
+      </c>
+      <c r="CE50" s="4" t="s">
+        <v>3915</v>
+      </c>
+      <c r="CF50" s="4" t="s">
+        <v>3934</v>
+      </c>
+      <c r="CG50" s="4" t="s">
+        <v>3962</v>
+      </c>
+      <c r="CH50" s="4" t="s">
+        <v>3987</v>
+      </c>
+      <c r="CI50" s="10"/>
       <c r="ATO50" s="1"/>
       <c r="ATP50" s="8"/>
       <c r="ATQ50" s="8"/>
@@ -60310,7 +62709,7 @@
       <c r="ATS50" s="7"/>
       <c r="ATT50" s="3"/>
     </row>
-    <row r="51" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>2472</v>
       </c>
@@ -60472,6 +62871,36 @@
       <c r="BU51" s="11" t="s">
         <v>3629</v>
       </c>
+      <c r="BV51" s="4" t="s">
+        <v>3759</v>
+      </c>
+      <c r="BW51" s="4" t="s">
+        <v>3784</v>
+      </c>
+      <c r="BZ51" s="4" t="s">
+        <v>3842</v>
+      </c>
+      <c r="CB51" s="4" t="s">
+        <v>3868</v>
+      </c>
+      <c r="CD51" s="4" t="s">
+        <v>3899</v>
+      </c>
+      <c r="CE51" s="4" t="s">
+        <v>3916</v>
+      </c>
+      <c r="CF51" s="4" t="s">
+        <v>3935</v>
+      </c>
+      <c r="CG51" s="4" t="s">
+        <v>3963</v>
+      </c>
+      <c r="CH51" s="4" t="s">
+        <v>3988</v>
+      </c>
+      <c r="CI51" s="4" t="s">
+        <v>4012</v>
+      </c>
       <c r="ATO51" s="1"/>
       <c r="ATP51" s="9"/>
       <c r="ATQ51" s="8"/>
@@ -60479,7 +62908,7 @@
       <c r="ATS51" s="6"/>
       <c r="ATT51" s="3"/>
     </row>
-    <row r="52" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>2522</v>
       </c>
@@ -60648,6 +63077,42 @@
       </c>
       <c r="BT52" s="4" t="s">
         <v>3621</v>
+      </c>
+      <c r="BV52" s="4" t="s">
+        <v>3747</v>
+      </c>
+      <c r="BW52" s="4" t="s">
+        <v>3785</v>
+      </c>
+      <c r="BX52" s="4" t="s">
+        <v>3807</v>
+      </c>
+      <c r="BY52" s="4" t="s">
+        <v>3824</v>
+      </c>
+      <c r="BZ52" s="4" t="s">
+        <v>3850</v>
+      </c>
+      <c r="CB52" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD52" s="11" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE52" s="11" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF52" s="11" t="s">
+        <v>3936</v>
+      </c>
+      <c r="CG52" s="4" t="s">
+        <v>3951</v>
+      </c>
+      <c r="CH52" s="4" t="s">
+        <v>3976</v>
+      </c>
+      <c r="CI52" s="4" t="s">
+        <v>4003</v>
       </c>
       <c r="ATO52" s="1"/>
       <c r="ATP52" s="8"/>
@@ -60656,7 +63121,7 @@
       <c r="ATS52" s="7"/>
       <c r="ATT52" s="3"/>
     </row>
-    <row r="53" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>2523</v>
       </c>
@@ -60823,6 +63288,42 @@
       </c>
       <c r="BT53" s="4" t="s">
         <v>3621</v>
+      </c>
+      <c r="BV53" s="4" t="s">
+        <v>3748</v>
+      </c>
+      <c r="BW53" s="4" t="s">
+        <v>3773</v>
+      </c>
+      <c r="BX53" s="4" t="s">
+        <v>3807</v>
+      </c>
+      <c r="BY53" s="4" t="s">
+        <v>3824</v>
+      </c>
+      <c r="BZ53" s="4" t="s">
+        <v>3850</v>
+      </c>
+      <c r="CB53" s="4" t="s">
+        <v>3865</v>
+      </c>
+      <c r="CD53" s="11" t="s">
+        <v>3892</v>
+      </c>
+      <c r="CE53" s="11" t="s">
+        <v>3909</v>
+      </c>
+      <c r="CF53" s="11" t="s">
+        <v>3936</v>
+      </c>
+      <c r="CG53" s="4" t="s">
+        <v>3952</v>
+      </c>
+      <c r="CH53" s="4" t="s">
+        <v>3989</v>
+      </c>
+      <c r="CI53" s="4" t="s">
+        <v>4004</v>
       </c>
       <c r="ATP53" s="8"/>
       <c r="ATQ53" s="8"/>
@@ -60830,7 +63331,7 @@
       <c r="ATS53" s="7"/>
       <c r="ATT53" s="3"/>
     </row>
-    <row r="54" spans="1:73 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:88 1211:1216" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>2524</v>
       </c>
@@ -60904,13 +63405,38 @@
       <c r="BO54" s="10"/>
       <c r="BQ54" s="10"/>
       <c r="BT54" s="10"/>
+      <c r="BV54" s="4" t="s">
+        <v>3760</v>
+      </c>
+      <c r="BW54" s="4" t="s">
+        <v>3786</v>
+      </c>
+      <c r="BX54" s="10"/>
+      <c r="BY54" s="10"/>
+      <c r="BZ54" s="10"/>
+      <c r="CA54" s="11" t="s">
+        <v>3852</v>
+      </c>
+      <c r="CB54" s="10"/>
+      <c r="CC54" s="11" t="s">
+        <v>3876</v>
+      </c>
+      <c r="CG54" s="11" t="s">
+        <v>3964</v>
+      </c>
+      <c r="CH54" s="11" t="s">
+        <v>3990</v>
+      </c>
+      <c r="CI54" s="11" t="s">
+        <v>4013</v>
+      </c>
       <c r="ATP54" s="7"/>
       <c r="ATQ54" s="7"/>
       <c r="ATR54" s="7"/>
       <c r="ATS54" s="7"/>
       <c r="ATT54" s="7"/>
     </row>
-    <row r="55" spans="1:73 1211:1216" ht="144.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:88 1211:1216" ht="144.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>2473</v>
       </c>
@@ -60972,6 +63498,24 @@
       <c r="BT55" s="4" t="s">
         <v>3605</v>
       </c>
+      <c r="BV55" s="4" t="s">
+        <v>3745</v>
+      </c>
+      <c r="BW55" s="4" t="s">
+        <v>3764</v>
+      </c>
+      <c r="BX55" s="4" t="s">
+        <v>3795</v>
+      </c>
+      <c r="BY55" s="4" t="s">
+        <v>3812</v>
+      </c>
+      <c r="BZ55" s="4" t="s">
+        <v>3834</v>
+      </c>
+      <c r="CB55" s="4" t="s">
+        <v>3875</v>
+      </c>
       <c r="ATO55" s="1"/>
       <c r="ATP55" s="7"/>
       <c r="ATQ55" s="7"/>
@@ -60979,7 +63523,7 @@
       <c r="ATS55" s="7"/>
       <c r="ATT55" s="7"/>
     </row>
-    <row r="56" spans="1:73 1211:1216" ht="247" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:88 1211:1216" ht="247" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>2474</v>
       </c>
@@ -61041,6 +63585,24 @@
       <c r="BT56" s="11" t="s">
         <v>3622</v>
       </c>
+      <c r="BV56" s="11" t="s">
+        <v>3741</v>
+      </c>
+      <c r="BW56" s="11" t="s">
+        <v>3766</v>
+      </c>
+      <c r="BX56" s="11" t="s">
+        <v>3808</v>
+      </c>
+      <c r="BY56" s="11" t="s">
+        <v>3821</v>
+      </c>
+      <c r="BZ56" s="11" t="s">
+        <v>3851</v>
+      </c>
+      <c r="CB56" s="11" t="s">
+        <v>3859</v>
+      </c>
       <c r="ATO56" s="1"/>
       <c r="ATP56" s="7"/>
       <c r="ATQ56" s="7"/>
@@ -61048,7 +63610,7 @@
       <c r="ATS56" s="7"/>
       <c r="ATT56" s="7"/>
     </row>
-    <row r="57" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>2475</v>
       </c>
@@ -61087,7 +63649,7 @@
       <c r="ATS57" s="6"/>
       <c r="ATT57" s="7"/>
     </row>
-    <row r="58" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>2476</v>
       </c>
@@ -61126,22 +63688,22 @@
       <c r="ATS58" s="6"/>
       <c r="ATT58" s="7"/>
     </row>
-    <row r="59" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="AR59" s="1"/>
     </row>
-    <row r="61" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:73 1211:1216" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:88 1211:1216" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="E64" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added buttons to change the form of pokemon, along with missed pokemon information
</commit_message>
<xml_diff>
--- a/Pokemonstuff2.xlsx
+++ b/Pokemonstuff2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f5c6edd2c1ca723/Documents/pokedex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5564" documentId="8_{6427532F-30D5-4B25-B377-222758C656F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F96EF276-568E-43AD-AD9F-815D243AD739}"/>
+  <xr:revisionPtr revIDLastSave="5578" documentId="8_{6427532F-30D5-4B25-B377-222758C656F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E35C79D-326B-4421-AF6E-05F949CB0428}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10283" uniqueCount="5983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10297" uniqueCount="5997">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -18455,6 +18455,48 @@
   <si>
     <t>Inner Focus
 Multiscale</t>
+  </si>
+  <si>
+    <t>Alola is the best environment for this Pokémon. Local people take pride in its appearance, saying this is how Exeggutor ought to look.</t>
+  </si>
+  <si>
+    <t>As it grew taller and taller, it outgrew its reliance on psychic powers, while within it awakened the power of the sleeping dragon.</t>
+  </si>
+  <si>
+    <t>Exeggutor is the pride of the Alolan people. Its image is carved into historical buildings and murals.</t>
+  </si>
+  <si>
+    <t>It swings its long neck like a whip and smacks its opponents. This makes Exeggutor itself dizzy, too.</t>
+  </si>
+  <si>
+    <t>The strong sunlight of the Alola region has awakened the power hidden within Exeggcute. This is the result.</t>
+  </si>
+  <si>
+    <t>Blazing sunlight has brought out the true form and powers of this Pokémon.</t>
+  </si>
+  <si>
+    <t>This Pokémon’s psychic powers aren’t as strong as they once were. The head on this Exeggutor’s tail scans surrounding areas with weak telepathy.</t>
+  </si>
+  <si>
+    <t>The bones it possesses were once its mother’s. Its mother’s regrets have become like a vengeful spirit protecting this Pokémon.</t>
+  </si>
+  <si>
+    <t>Its custom is to mourn its lost companions. Mounds of dirt by the side of the road mark the graves of the Marowak.</t>
+  </si>
+  <si>
+    <t>The rich greenery of the Alola region is hard on Marowak. It controls fire to stay alive.</t>
+  </si>
+  <si>
+    <t>When it beats opponents with its bone, the cursed flames spread to them. No amount of water will stop those flames from burning.</t>
+  </si>
+  <si>
+    <t>It has transformed the spirit of its dear departed mother into flames, and tonight it will once again dance in mourning of others of its kind.</t>
+  </si>
+  <si>
+    <t>This Pokémon sets the bone it holds on fire and dances through the night as a way to mourn its fallen allies.</t>
+  </si>
+  <si>
+    <t>The cursed flames that light up the bone carried by this Pokémon are said to cause both mental and physical pain that will never fade.</t>
   </si>
 </sst>
 </file>
@@ -19488,9 +19530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ATT1216"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="GP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="GW13" sqref="GW13"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="EH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EN52" sqref="EN52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -76717,11 +76759,17 @@
       <c r="EJ45" s="16" t="s">
         <v>4509</v>
       </c>
+      <c r="EK45" s="4" t="s">
+        <v>5983</v>
+      </c>
       <c r="EL45" s="16" t="s">
         <v>4528</v>
       </c>
       <c r="EM45" s="16" t="s">
         <v>4545</v>
+      </c>
+      <c r="EN45" s="4" t="s">
+        <v>5990</v>
       </c>
       <c r="EW45" s="15" t="s">
         <v>4682</v>
@@ -77055,11 +77103,17 @@
       <c r="EJ46" s="15" t="s">
         <v>4510</v>
       </c>
+      <c r="EK46" s="4" t="s">
+        <v>5984</v>
+      </c>
       <c r="EL46" s="15" t="s">
         <v>4529</v>
       </c>
       <c r="EM46" s="15" t="s">
         <v>4546</v>
+      </c>
+      <c r="EN46" s="4" t="s">
+        <v>5991</v>
       </c>
       <c r="EW46" s="16" t="s">
         <v>4683</v>
@@ -77402,11 +77456,17 @@
       <c r="EJ47" s="16" t="s">
         <v>4511</v>
       </c>
+      <c r="EK47" s="4" t="s">
+        <v>5985</v>
+      </c>
       <c r="EL47" s="16" t="s">
         <v>4530</v>
       </c>
       <c r="EM47" s="16" t="s">
         <v>4547</v>
+      </c>
+      <c r="EN47" s="4" t="s">
+        <v>5992</v>
       </c>
       <c r="EQ47" s="16" t="s">
         <v>4592</v>
@@ -77770,11 +77830,17 @@
       <c r="EJ48" s="15" t="s">
         <v>4512</v>
       </c>
+      <c r="EK48" s="4" t="s">
+        <v>5986</v>
+      </c>
       <c r="EL48" s="15" t="s">
         <v>4531</v>
       </c>
       <c r="EM48" s="15" t="s">
         <v>4548</v>
+      </c>
+      <c r="EN48" s="4" t="s">
+        <v>5993</v>
       </c>
       <c r="EQ48" s="15" t="s">
         <v>4593</v>
@@ -78271,11 +78337,17 @@
       <c r="EJ49" s="16" t="s">
         <v>4513</v>
       </c>
+      <c r="EK49" s="4" t="s">
+        <v>5987</v>
+      </c>
       <c r="EL49" s="16" t="s">
         <v>4518</v>
       </c>
       <c r="EM49" s="16" t="s">
         <v>4549</v>
+      </c>
+      <c r="EN49" s="4" t="s">
+        <v>5994</v>
       </c>
       <c r="EO49" s="16" t="s">
         <v>4554</v>
@@ -78725,11 +78797,17 @@
       <c r="EJ50" s="15" t="s">
         <v>4514</v>
       </c>
+      <c r="EK50" s="4" t="s">
+        <v>5988</v>
+      </c>
       <c r="EL50" s="15" t="s">
         <v>4532</v>
       </c>
       <c r="EM50" s="15" t="s">
         <v>4550</v>
+      </c>
+      <c r="EN50" s="4" t="s">
+        <v>5995</v>
       </c>
       <c r="EO50" s="15" t="s">
         <v>4563</v>
@@ -79158,11 +79236,17 @@
       <c r="EJ51" s="16" t="s">
         <v>4515</v>
       </c>
+      <c r="EK51" s="11" t="s">
+        <v>5989</v>
+      </c>
       <c r="EL51" s="16" t="s">
         <v>4533</v>
       </c>
       <c r="EM51" s="16" t="s">
         <v>4551</v>
+      </c>
+      <c r="EN51" s="11" t="s">
+        <v>5996</v>
       </c>
       <c r="EO51" s="16" t="s">
         <v>4559</v>

</xml_diff>